<commit_message>
feat(gms/preprocessing): boundary sector storage introduced
Added new boundary sector specific input files and changed config files
</commit_message>
<xml_diff>
--- a/ConfigFiles/ConfigTestBoundarySector.xlsx
+++ b/ConfigFiles/ConfigTestBoundarySector.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24827"/>
   <workbookPr updateLinks="never" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\Github\Dispa-SET.git\ConfigFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02C63CB9-9A0B-41B5-80CB-0B6A476CC01B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A05D9C3-E039-42E2-A9B8-336B64E6201D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="249">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="251">
   <si>
     <t>Default value</t>
   </si>
@@ -783,6 +783,12 @@
   </si>
   <si>
     <t>Price of Userved Boundary Sector</t>
+  </si>
+  <si>
+    <t>Boundary Sector Inputs</t>
+  </si>
+  <si>
+    <t>tests/dummy_data/boundary_sector/BoundarySectorInputs.csv</t>
   </si>
 </sst>
 </file>
@@ -1539,8 +1545,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:H330"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A74" workbookViewId="0">
-      <selection activeCell="C141" sqref="C141"/>
+    <sheetView tabSelected="1" topLeftCell="A101" workbookViewId="0">
+      <selection activeCell="C143" sqref="C143"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2352,11 +2358,18 @@
         <v>247</v>
       </c>
     </row>
-    <row r="142" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A142" s="25"/>
-      <c r="C142" s="27"/>
-    </row>
-    <row r="143" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:8" s="26" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A142" s="25" t="s">
+        <v>249</v>
+      </c>
+      <c r="B142" s="29" t="s">
+        <v>35</v>
+      </c>
+      <c r="C142" s="19" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="143" spans="1:8" s="26" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A143" s="25"/>
       <c r="C143" s="27"/>
     </row>
@@ -2424,7 +2437,7 @@
       <c r="A159" s="25"/>
       <c r="C159" s="27"/>
     </row>
-    <row r="160" spans="1:3" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:3" s="26" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A160" s="25"/>
       <c r="C160" s="27"/>
     </row>

</xml_diff>

<commit_message>
feat(bs_ntc): added flows between boundary sectors
</commit_message>
<xml_diff>
--- a/ConfigFiles/ConfigTestBoundarySector.xlsx
+++ b/ConfigFiles/ConfigTestBoundarySector.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\Github\Dispa-SET.git\ConfigFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F982D9C9-6085-4E8D-9288-A004ACCF62B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE658855-7707-466D-88F1-AB4A9BA97406}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="251">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="255">
   <si>
     <t>Default value</t>
   </si>
@@ -789,6 +789,18 @@
   </si>
   <si>
     <t>tests/dummy_data/boundary_sector/BoundarySectorInputs.csv</t>
+  </si>
+  <si>
+    <t>Boundary Sector NTC</t>
+  </si>
+  <si>
+    <t>Boundary Sector Historical Flows</t>
+  </si>
+  <si>
+    <t>tests/dummy_data/boundary_sector/BS_NTCs.csv</t>
+  </si>
+  <si>
+    <t>tests/dummy_data/boundary_sector/BS_CBFs.csv</t>
   </si>
 </sst>
 </file>
@@ -1545,8 +1557,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:H330"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A131" workbookViewId="0">
-      <selection activeCell="C134" sqref="C134"/>
+    <sheetView tabSelected="1" topLeftCell="A124" workbookViewId="0">
+      <selection activeCell="G139" sqref="G139"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2370,14 +2382,28 @@
       </c>
     </row>
     <row r="143" spans="1:8" s="26" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A143" s="25"/>
-      <c r="C143" s="27"/>
-    </row>
-    <row r="144" spans="1:8" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A144" s="25"/>
-      <c r="C144" s="27"/>
-    </row>
-    <row r="145" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A143" s="25" t="s">
+        <v>251</v>
+      </c>
+      <c r="B143" s="29" t="s">
+        <v>35</v>
+      </c>
+      <c r="C143" s="19" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="144" spans="1:8" s="26" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A144" s="25" t="s">
+        <v>252</v>
+      </c>
+      <c r="B144" s="29" t="s">
+        <v>35</v>
+      </c>
+      <c r="C144" s="19" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3" s="26" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A145" s="25"/>
       <c r="C145" s="27"/>
     </row>

</xml_diff>

<commit_message>
feat(BS flexible demand): added flexible demand to the boundary sector
</commit_message>
<xml_diff>
--- a/ConfigFiles/ConfigTestBoundarySector.xlsx
+++ b/ConfigFiles/ConfigTestBoundarySector.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\Github\Dispa-SET.git\ConfigFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE658855-7707-466D-88F1-AB4A9BA97406}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67591B8C-E875-443E-9571-A7657BBD036B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="255">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="259">
   <si>
     <t>Default value</t>
   </si>
@@ -801,6 +801,18 @@
   </si>
   <si>
     <t>tests/dummy_data/boundary_sector/BS_CBFs.csv</t>
+  </si>
+  <si>
+    <t>tests/dummy_data/boundary_sector/BSFlexibleDemand.csv</t>
+  </si>
+  <si>
+    <t>tests/dummy_data/boundary_sector/BSFlexibleCapacities.csv</t>
+  </si>
+  <si>
+    <t>Boundary Sector Demand (flexible)</t>
+  </si>
+  <si>
+    <t>Boundary Sector Capacity (flexible)</t>
   </si>
 </sst>
 </file>
@@ -1557,13 +1569,13 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:H330"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A124" workbookViewId="0">
-      <selection activeCell="G139" sqref="G139"/>
+    <sheetView tabSelected="1" topLeftCell="A123" workbookViewId="0">
+      <selection activeCell="C145" sqref="C145"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.5703125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="48.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.42578125" style="1" customWidth="1"/>
     <col min="3" max="3" width="68.7109375" style="13" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6.140625" style="1" customWidth="1"/>
@@ -2404,14 +2416,28 @@
       </c>
     </row>
     <row r="145" spans="1:3" s="26" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A145" s="25"/>
-      <c r="C145" s="27"/>
-    </row>
-    <row r="146" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A146" s="25"/>
-      <c r="C146" s="27"/>
-    </row>
-    <row r="147" spans="1:3" s="26" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A145" s="25" t="s">
+        <v>257</v>
+      </c>
+      <c r="B145" s="29" t="s">
+        <v>35</v>
+      </c>
+      <c r="C145" s="19" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3" s="26" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A146" s="25" t="s">
+        <v>258</v>
+      </c>
+      <c r="B146" s="29" t="s">
+        <v>35</v>
+      </c>
+      <c r="C146" s="19" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3" s="26" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A147" s="25"/>
       <c r="C147" s="27"/>
     </row>
@@ -4055,7 +4081,7 @@
       <formula>NOT(ISERROR(SEARCH("TRUE",F313)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations xWindow="547" yWindow="733" count="35">
+  <dataValidations disablePrompts="1" xWindow="547" yWindow="733" count="35">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Path the simulation directory" prompt="All inputs are saved in the so-called simulation directory, which includes, excel , gdx and pickle files together with the GAMS files._x000a__x000a_The path should be relative to this excel file. Use &quot;..&quot; to go up one folder. Folder separator can be either &quot;/&quot; or &quot;\&quot;" sqref="C34:D34" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
     <dataValidation type="date" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Start day of the simulation" prompt="This is the simulated day. It must be comprised within the range of dates provided within the data files." sqref="C57" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>1</formula1>
@@ -4108,7 +4134,7 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xWindow="547" yWindow="733" count="9">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" xWindow="547" yWindow="733" count="9">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000011000000}">
           <x14:formula1>
             <xm:f>Lists!$A$2:$A$3</xm:f>

</xml_diff>

<commit_message>
fix(all_bs): h2 sector removed, can be entirely modeled with boundary sector units
</commit_message>
<xml_diff>
--- a/ConfigFiles/ConfigTestBoundarySector.xlsx
+++ b/ConfigFiles/ConfigTestBoundarySector.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\Github\Dispa-SET.git\ConfigFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67591B8C-E875-443E-9571-A7657BBD036B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23740932-4305-485F-B5D9-FE2468345C62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="259">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="255">
   <si>
     <t>Default value</t>
   </si>
@@ -671,24 +671,9 @@
     <t>Reserves Up</t>
   </si>
   <si>
-    <t>Price of Unserved H2</t>
-  </si>
-  <si>
-    <t>Geo Data</t>
-  </si>
-  <si>
     <t>tests/dummy_data/Geo_Coordinates.csv</t>
   </si>
   <si>
-    <t>H2 Demand (P2H2 - rigid)</t>
-  </si>
-  <si>
-    <t>H2 Demand (P2Liquid - flexible)</t>
-  </si>
-  <si>
-    <t>H2 Capacities (P2Liquid - flexible)</t>
-  </si>
-  <si>
     <t>ZZ3</t>
   </si>
   <si>
@@ -782,9 +767,6 @@
     <t>tests/dummy_data/boundary_sector/BoundarySectorDemand.csv</t>
   </si>
   <si>
-    <t>Price of Userved Boundary Sector</t>
-  </si>
-  <si>
     <t>Boundary Sector Inputs</t>
   </si>
   <si>
@@ -813,6 +795,12 @@
   </si>
   <si>
     <t>Boundary Sector Capacity (flexible)</t>
+  </si>
+  <si>
+    <t>GeoData (geographical coordinates)</t>
+  </si>
+  <si>
+    <t>Price of Userved Energy in the Boundary Sector</t>
   </si>
 </sst>
 </file>
@@ -973,7 +961,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1104,6 +1092,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1569,8 +1560,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:H330"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A123" workbookViewId="0">
-      <selection activeCell="C145" sqref="C145"/>
+    <sheetView tabSelected="1" topLeftCell="A101" workbookViewId="0">
+      <selection activeCell="C129" sqref="C129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1587,16 +1578,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="47" t="s">
-        <v>245</v>
-      </c>
-      <c r="B1" s="47"/>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
-      <c r="F1" s="47"/>
-      <c r="G1" s="47"/>
-      <c r="H1" s="47"/>
+      <c r="A1" s="48" t="s">
+        <v>240</v>
+      </c>
+      <c r="B1" s="48"/>
+      <c r="C1" s="48"/>
+      <c r="D1" s="48"/>
+      <c r="E1" s="48"/>
+      <c r="F1" s="48"/>
+      <c r="G1" s="48"/>
+      <c r="H1" s="48"/>
     </row>
     <row r="2" spans="1:8" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
@@ -1611,15 +1602,15 @@
     <row r="3" spans="1:8" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="1:8" s="34" customFormat="1" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="33"/>
-      <c r="B4" s="48" t="s">
+      <c r="B4" s="49" t="s">
         <v>56</v>
       </c>
-      <c r="C4" s="48"/>
-      <c r="D4" s="48"/>
-      <c r="E4" s="48"/>
-      <c r="F4" s="48"/>
-      <c r="G4" s="48"/>
-      <c r="H4" s="48"/>
+      <c r="C4" s="49"/>
+      <c r="D4" s="49"/>
+      <c r="E4" s="49"/>
+      <c r="F4" s="49"/>
+      <c r="G4" s="49"/>
+      <c r="H4" s="49"/>
     </row>
     <row r="5" spans="1:8" s="8" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="7"/>
@@ -1635,15 +1626,15 @@
       <c r="A6" s="39" t="s">
         <v>49</v>
       </c>
-      <c r="B6" s="45" t="s">
+      <c r="B6" s="46" t="s">
         <v>181</v>
       </c>
-      <c r="C6" s="45"/>
-      <c r="D6" s="45"/>
-      <c r="E6" s="45"/>
-      <c r="F6" s="45"/>
-      <c r="G6" s="45"/>
-      <c r="H6" s="45"/>
+      <c r="C6" s="46"/>
+      <c r="D6" s="46"/>
+      <c r="E6" s="46"/>
+      <c r="F6" s="46"/>
+      <c r="G6" s="46"/>
+      <c r="H6" s="46"/>
     </row>
     <row r="7" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="44"/>
@@ -1781,7 +1772,7 @@
         <v>35</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="D34" s="13"/>
       <c r="H34" s="1" t="s">
@@ -1990,7 +1981,7 @@
         <v>59</v>
       </c>
       <c r="C78" s="4" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="H78" s="1" t="s">
         <v>64</v>
@@ -2202,7 +2193,7 @@
         <v>35</v>
       </c>
       <c r="C128" s="19" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
       <c r="D128" s="18" t="s">
         <v>87</v>
@@ -2332,13 +2323,13 @@
     </row>
     <row r="137" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A137" s="2" t="s">
-        <v>212</v>
+        <v>253</v>
       </c>
       <c r="B137" s="29" t="s">
         <v>35</v>
       </c>
       <c r="C137" s="19" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="D137" s="18" t="s">
         <v>87</v>
@@ -2346,30 +2337,36 @@
     </row>
     <row r="138" spans="1:8" s="26" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A138" s="25" t="s">
-        <v>214</v>
+        <v>241</v>
       </c>
       <c r="B138" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="C138" s="19"/>
+      <c r="C138" s="19" t="s">
+        <v>242</v>
+      </c>
     </row>
     <row r="139" spans="1:8" s="26" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A139" s="25" t="s">
-        <v>215</v>
+        <v>243</v>
       </c>
       <c r="B139" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="C139" s="19"/>
+      <c r="C139" s="19" t="s">
+        <v>244</v>
+      </c>
     </row>
     <row r="140" spans="1:8" s="26" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A140" s="25" t="s">
-        <v>216</v>
+        <v>245</v>
       </c>
       <c r="B140" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="C140" s="19"/>
+      <c r="C140" s="19" t="s">
+        <v>247</v>
+      </c>
     </row>
     <row r="141" spans="1:8" s="26" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A141" s="25" t="s">
@@ -2379,63 +2376,45 @@
         <v>35</v>
       </c>
       <c r="C141" s="19" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
     </row>
     <row r="142" spans="1:8" s="26" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A142" s="25" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="B142" s="29" t="s">
         <v>35</v>
       </c>
       <c r="C142" s="19" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="143" spans="1:8" s="26" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A143" s="25" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="B143" s="29" t="s">
         <v>35</v>
       </c>
       <c r="C143" s="19" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
     </row>
     <row r="144" spans="1:8" s="26" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A144" s="25" t="s">
-        <v>252</v>
-      </c>
-      <c r="B144" s="29" t="s">
-        <v>35</v>
-      </c>
-      <c r="C144" s="19" t="s">
-        <v>254</v>
-      </c>
+      <c r="A144" s="25"/>
+      <c r="B144" s="1"/>
+      <c r="C144" s="45"/>
     </row>
     <row r="145" spans="1:3" s="26" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A145" s="25" t="s">
-        <v>257</v>
-      </c>
-      <c r="B145" s="29" t="s">
-        <v>35</v>
-      </c>
-      <c r="C145" s="19" t="s">
-        <v>255</v>
-      </c>
+      <c r="A145" s="25"/>
+      <c r="B145" s="1"/>
+      <c r="C145" s="45"/>
     </row>
     <row r="146" spans="1:3" s="26" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A146" s="25" t="s">
-        <v>258</v>
-      </c>
-      <c r="B146" s="29" t="s">
-        <v>35</v>
-      </c>
-      <c r="C146" s="19" t="s">
-        <v>256</v>
-      </c>
+      <c r="A146" s="25"/>
+      <c r="B146" s="1"/>
+      <c r="C146" s="45"/>
     </row>
     <row r="147" spans="1:3" s="26" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A147" s="25"/>
@@ -2635,8 +2614,8 @@
       </c>
     </row>
     <row r="171" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A171" s="2" t="s">
-        <v>211</v>
+      <c r="A171" s="25" t="s">
+        <v>254</v>
       </c>
       <c r="B171" s="29" t="s">
         <v>35</v>
@@ -2654,7 +2633,7 @@
     </row>
     <row r="172" spans="1:8" s="26" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A172" s="2" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="B172" s="29" t="s">
         <v>35</v>
@@ -2670,24 +2649,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="173" spans="1:8" s="26" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A173" s="25" t="s">
-        <v>248</v>
-      </c>
-      <c r="B173" s="29" t="s">
-        <v>35</v>
-      </c>
-      <c r="C173" s="19"/>
-      <c r="D173" s="18" t="s">
-        <v>87</v>
-      </c>
-      <c r="E173" s="28" t="s">
-        <v>0</v>
-      </c>
-      <c r="F173" s="5">
-        <v>110000</v>
-      </c>
-    </row>
+    <row r="173" spans="1:8" s="26" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="174" spans="1:8" s="26" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A174" s="25"/>
       <c r="C174" s="27"/>
@@ -2855,7 +2817,7 @@
     </row>
     <row r="188" spans="1:8" s="26" customFormat="1" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A188" s="25" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="B188" s="29" t="s">
         <v>35</v>
@@ -3082,7 +3044,7 @@
       </c>
     </row>
     <row r="227" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A227" s="46" t="s">
+      <c r="A227" s="47" t="s">
         <v>51</v>
       </c>
       <c r="B227" s="6" t="s">
@@ -3095,7 +3057,7 @@
         <v>1</v>
       </c>
       <c r="E227" s="6" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="F227" s="4" t="b">
         <v>0</v>
@@ -3105,7 +3067,7 @@
       </c>
     </row>
     <row r="228" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A228" s="46"/>
+      <c r="A228" s="47"/>
       <c r="B228" s="6" t="s">
         <v>21</v>
       </c>
@@ -3126,7 +3088,7 @@
       </c>
     </row>
     <row r="229" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A229" s="46"/>
+      <c r="A229" s="47"/>
       <c r="B229" s="6" t="s">
         <v>149</v>
       </c>
@@ -3147,7 +3109,7 @@
       </c>
     </row>
     <row r="230" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A230" s="46"/>
+      <c r="A230" s="47"/>
       <c r="B230" s="6" t="s">
         <v>131</v>
       </c>
@@ -3168,7 +3130,7 @@
       </c>
     </row>
     <row r="231" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A231" s="46"/>
+      <c r="A231" s="47"/>
       <c r="B231" s="6" t="s">
         <v>5</v>
       </c>
@@ -3189,7 +3151,7 @@
       </c>
     </row>
     <row r="232" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A232" s="46"/>
+      <c r="A232" s="47"/>
       <c r="B232" s="6" t="s">
         <v>152</v>
       </c>
@@ -3210,7 +3172,7 @@
       </c>
     </row>
     <row r="233" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A233" s="46"/>
+      <c r="A233" s="47"/>
       <c r="B233" s="6" t="s">
         <v>30</v>
       </c>
@@ -3231,7 +3193,7 @@
       </c>
     </row>
     <row r="234" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A234" s="46"/>
+      <c r="A234" s="47"/>
       <c r="B234" s="6" t="s">
         <v>16</v>
       </c>
@@ -3252,7 +3214,7 @@
       </c>
     </row>
     <row r="235" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A235" s="46"/>
+      <c r="A235" s="47"/>
       <c r="B235" s="6" t="s">
         <v>6</v>
       </c>
@@ -3273,7 +3235,7 @@
       </c>
     </row>
     <row r="236" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A236" s="46"/>
+      <c r="A236" s="47"/>
       <c r="B236" s="6" t="s">
         <v>8</v>
       </c>
@@ -3294,7 +3256,7 @@
       </c>
     </row>
     <row r="237" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A237" s="46"/>
+      <c r="A237" s="47"/>
       <c r="B237" s="6" t="s">
         <v>7</v>
       </c>
@@ -3315,7 +3277,7 @@
       </c>
     </row>
     <row r="238" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A238" s="46"/>
+      <c r="A238" s="47"/>
       <c r="B238" s="6" t="s">
         <v>9</v>
       </c>
@@ -3336,7 +3298,7 @@
       </c>
     </row>
     <row r="239" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A239" s="46"/>
+      <c r="A239" s="47"/>
       <c r="B239" s="6" t="s">
         <v>11</v>
       </c>
@@ -3357,7 +3319,7 @@
       </c>
     </row>
     <row r="240" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A240" s="46"/>
+      <c r="A240" s="47"/>
       <c r="B240" s="6" t="s">
         <v>12</v>
       </c>
@@ -3378,7 +3340,7 @@
       </c>
     </row>
     <row r="241" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A241" s="46"/>
+      <c r="A241" s="47"/>
       <c r="B241" s="6" t="s">
         <v>27</v>
       </c>
@@ -3459,7 +3421,7 @@
       </c>
     </row>
     <row r="245" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A245" s="49" t="s">
+      <c r="A245" s="50" t="s">
         <v>170</v>
       </c>
       <c r="B245" s="6" t="s">
@@ -3482,7 +3444,7 @@
       </c>
     </row>
     <row r="246" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A246" s="49"/>
+      <c r="A246" s="50"/>
       <c r="B246" s="6" t="s">
         <v>158</v>
       </c>
@@ -3708,7 +3670,7 @@
     </row>
     <row r="299" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A299" s="2" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="C299" s="31" t="s">
         <v>4</v>
@@ -3775,7 +3737,7 @@
     </row>
     <row r="305" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A305" s="2" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="C305" s="31" t="s">
         <v>4</v>
@@ -3792,7 +3754,7 @@
         <v>1</v>
       </c>
       <c r="E306" s="22" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="F306" s="21" t="b">
         <v>1</v>
@@ -3806,7 +3768,7 @@
         <v>1</v>
       </c>
       <c r="E307" s="22" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="F307" s="21" t="b">
         <v>1</v>
@@ -3820,7 +3782,7 @@
         <v>1</v>
       </c>
       <c r="E308" s="22" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="F308" s="21" t="b">
         <v>1</v>
@@ -3834,7 +3796,7 @@
         <v>0</v>
       </c>
       <c r="E309" s="22" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="F309" s="21" t="b">
         <v>1</v>
@@ -3848,7 +3810,7 @@
         <v>1</v>
       </c>
       <c r="E310" s="22" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="F310" s="21" t="b">
         <v>1</v>
@@ -3862,7 +3824,7 @@
         <v>1</v>
       </c>
       <c r="E311" s="22" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="F311" s="21" t="b">
         <v>1</v>
@@ -3876,7 +3838,7 @@
         <v>0</v>
       </c>
       <c r="E312" s="22" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="F312" s="21" t="b">
         <v>1</v>
@@ -3890,7 +3852,7 @@
         <v>0</v>
       </c>
       <c r="E313" s="22" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="F313" s="21" t="b">
         <v>0</v>
@@ -3904,7 +3866,7 @@
         <v>0</v>
       </c>
       <c r="E314" s="22" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="F314" s="21" t="b">
         <v>0</v>
@@ -3918,7 +3880,7 @@
         <v>0</v>
       </c>
       <c r="E315" s="22" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="F315" s="21" t="b">
         <v>0</v>
@@ -3932,7 +3894,7 @@
         <v>1</v>
       </c>
       <c r="E316" s="22" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="F316" s="21" t="b">
         <v>0</v>
@@ -3946,7 +3908,7 @@
         <v>1</v>
       </c>
       <c r="E317" s="22" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="F317" s="21" t="b">
         <v>0</v>
@@ -3960,7 +3922,7 @@
         <v>1</v>
       </c>
       <c r="E318" s="22" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="F318" s="21" t="b">
         <v>0</v>
@@ -3974,7 +3936,7 @@
         <v>0</v>
       </c>
       <c r="E319" s="22" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="F319" s="21" t="b">
         <v>0</v>
@@ -3988,7 +3950,7 @@
         <v>0</v>
       </c>
       <c r="E320" s="22" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="F320" s="21" t="b">
         <v>0</v>
@@ -3996,13 +3958,13 @@
     </row>
     <row r="321" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B321" s="22" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="C321" s="21" t="b">
         <v>0</v>
       </c>
       <c r="E321" s="22" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="F321" s="21" t="b">
         <v>0</v>
@@ -4010,7 +3972,7 @@
     </row>
     <row r="322" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E322" s="22" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="F322" s="21" t="b">
         <v>0</v>
@@ -4092,14 +4054,13 @@
       <formula2>73051</formula2>
     </dataValidation>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Historical interconnection flows" prompt="Historical flows" sqref="C132" xr:uid="{00000000-0002-0000-0000-000003000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Default value" prompt="In case no data file is provided. This single value is used for all the sets." sqref="F168 F181:F188 F171:F173" xr:uid="{00000000-0002-0000-0000-000004000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Default value" prompt="In case no data file is provided. This single value is used for all the sets." sqref="F168 F181:F188 F171:F172" xr:uid="{00000000-0002-0000-0000-000004000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Multiplicative Factor" prompt="This modifier multiplies the demand curves of all the zones by the provided factor" sqref="C275" xr:uid="{00000000-0002-0000-0000-000005000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Multiplicative Factor" prompt="This modifier multiplies the wind generation curves of all the zones by the provided factor" sqref="C276" xr:uid="{00000000-0002-0000-0000-000006000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Multiplicative Factor" prompt="This modifier multiplies the PV generation curves of all the zones by the provided factor" sqref="C277" xr:uid="{00000000-0002-0000-0000-000007000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Multiplicative Factor" prompt="This modifier multiplies the storage capacity in all the zones by the provided factor" sqref="C278" xr:uid="{00000000-0002-0000-0000-000008000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Path to the gams folder" prompt="Example:_x000a_C:\GAMS\win64\24.3_x000a__x000a_If unspecified or non-existing, Dispa-SET will try to determine the path automatically. " sqref="C37" xr:uid="{00000000-0002-0000-0000-000009000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Default value (% of max load)" prompt="In case no data file is provided. This single value is used for all the sets._x000a_It is defined in % of the maximum load throughout the simulation period." sqref="F130" xr:uid="{00000000-0002-0000-0000-00000A000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Default value (in EUR/t_co2)" prompt="In case no data file is provided. This single value is used for all the sets." sqref="F167:F173" xr:uid="{00000000-0002-0000-0000-00000B000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Path to the cplex executable" prompt="This is only useful if the Pyomo engine is selected and if cplex is not in the PATH (i.e. accessible from the prompt). This parameters can be left unspecified in most cases._x000a__x000a_Example:_x000a_C:\\Users\\ese-veda06\\Downloads\\solvers\\cplex.exe" sqref="C38" xr:uid="{00000000-0002-0000-0000-00000C000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Reservoir inflows in MWh" sqref="C133" xr:uid="{00000000-0002-0000-0000-00000D000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Path the outage data" prompt="Select the path the outage csv file from the database._x000a__x000a_The path should be relative to this excel file. Use &quot;..&quot; to go up one folder. Folder separator can be either &quot;/&quot; or &quot;\&quot;" sqref="C127" xr:uid="{00000000-0002-0000-0000-00000E000000}"/>
@@ -4128,7 +4089,8 @@
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Reserve down requirements" prompt="Path to the time series for each zone._x000a_The unit should be MW_x000a_If not provided, a standard formula is used to evaluate the reserve needs" sqref="C162" xr:uid="{094AD1A9-55C8-427E-B2FD-E6A9640F2346}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Reserve up requirements" prompt="Path to the time series for each zone._x000a_The unit should be MW_x000a_If not provided, a standard formula is used to evaluate the reserve needs" sqref="C161" xr:uid="{54B64FDA-AB14-4A05-907F-32559C9DD1CC}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Heating demand" prompt="expressed in MWh" sqref="C135" xr:uid="{F5C6CB55-A203-47FE-96B0-DC9C451014C9}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Demand for Hydrogen" prompt="Time series, expressed in MWh!" sqref="C137:C138" xr:uid="{CA14712D-8AB1-47D5-9826-5119B72CD67D}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Demand for Hydrogen" prompt="Time series, expressed in MWh!" sqref="C137" xr:uid="{CA14712D-8AB1-47D5-9826-5119B72CD67D}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Default value (in EUR/t_co2)" prompt="In case no data file is provided. This single value is used for all the sets." sqref="F167:F172" xr:uid="{00000000-0002-0000-0000-00000B000000}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4261,7 +4223,7 @@
         <v>43</v>
       </c>
       <c r="C3" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="D3" t="s">
         <v>83</v>
@@ -4278,7 +4240,7 @@
         <v>44</v>
       </c>
       <c r="C4" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="D4" t="s">
         <v>80</v>
@@ -4292,7 +4254,7 @@
         <v>130</v>
       </c>
       <c r="C5" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="D5" t="s">
         <v>81</v>

</xml_diff>

<commit_message>
fix(build): remove redundant h2 sector units, include BS spillage
</commit_message>
<xml_diff>
--- a/ConfigFiles/ConfigTestBoundarySector.xlsx
+++ b/ConfigFiles/ConfigTestBoundarySector.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25330"/>
   <workbookPr updateLinks="never" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\Github\Dispa-SET.git\ConfigFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23740932-4305-485F-B5D9-FE2468345C62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C86B7E1-7C14-4508-A54F-14C6CE94E675}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="255">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="257">
   <si>
     <t>Default value</t>
   </si>
@@ -755,24 +755,15 @@
     <t>Simulations/simulation_test_bs</t>
   </si>
   <si>
-    <t>tests/dummy_data/boundary_sector/Units_testcase.csv</t>
-  </si>
-  <si>
     <t>Dispa-SET Configuration File (v20.03)</t>
   </si>
   <si>
     <t>Boundary Sector Demand</t>
   </si>
   <si>
-    <t>tests/dummy_data/boundary_sector/BoundarySectorDemand.csv</t>
-  </si>
-  <si>
     <t>Boundary Sector Inputs</t>
   </si>
   <si>
-    <t>tests/dummy_data/boundary_sector/BoundarySectorInputs.csv</t>
-  </si>
-  <si>
     <t>Boundary Sector NTC</t>
   </si>
   <si>
@@ -785,12 +776,6 @@
     <t>tests/dummy_data/boundary_sector/BS_CBFs.csv</t>
   </si>
   <si>
-    <t>tests/dummy_data/boundary_sector/BSFlexibleDemand.csv</t>
-  </si>
-  <si>
-    <t>tests/dummy_data/boundary_sector/BSFlexibleCapacities.csv</t>
-  </si>
-  <si>
     <t>Boundary Sector Demand (flexible)</t>
   </si>
   <si>
@@ -801,6 +786,27 @@
   </si>
   <si>
     <t>Price of Userved Energy in the Boundary Sector</t>
+  </si>
+  <si>
+    <t>tests/dummy_data/boundary_sector/BS_Demand.csv</t>
+  </si>
+  <si>
+    <t>tests/dummy_data/boundary_sector/BS_Inputs.csv</t>
+  </si>
+  <si>
+    <t>tests/dummy_data/boundary_sector/BS_FlexibleDemand.csv</t>
+  </si>
+  <si>
+    <t>tests/dummy_data/boundary_sector/BS_FlexibleCapacities.csv</t>
+  </si>
+  <si>
+    <t>tests/dummy_data/boundary_sector/BS_Units_testcase.csv</t>
+  </si>
+  <si>
+    <t>tests/dummy_data/Temperatures.csv</t>
+  </si>
+  <si>
+    <t>tests/dummy_data/HeatDemand.csv</t>
   </si>
 </sst>
 </file>
@@ -1560,8 +1566,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:H330"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A101" workbookViewId="0">
-      <selection activeCell="C129" sqref="C129"/>
+    <sheetView tabSelected="1" topLeftCell="A237" workbookViewId="0">
+      <selection activeCell="C276" sqref="C276"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1579,7 +1585,7 @@
   <sheetData>
     <row r="1" spans="1:8" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="48" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B1" s="48"/>
       <c r="C1" s="48"/>
@@ -2193,7 +2199,7 @@
         <v>35</v>
       </c>
       <c r="C128" s="19" t="s">
-        <v>239</v>
+        <v>254</v>
       </c>
       <c r="D128" s="18" t="s">
         <v>87</v>
@@ -2303,7 +2309,9 @@
       <c r="B135" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="C135" s="19"/>
+      <c r="C135" s="19" t="s">
+        <v>256</v>
+      </c>
       <c r="D135" s="18" t="s">
         <v>87</v>
       </c>
@@ -2315,7 +2323,9 @@
       <c r="B136" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="C136" s="19"/>
+      <c r="C136" s="19" t="s">
+        <v>255</v>
+      </c>
       <c r="D136" s="18" t="s">
         <v>87</v>
       </c>
@@ -2323,7 +2333,7 @@
     </row>
     <row r="137" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A137" s="2" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="B137" s="29" t="s">
         <v>35</v>
@@ -2337,68 +2347,68 @@
     </row>
     <row r="138" spans="1:8" s="26" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A138" s="25" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B138" s="29" t="s">
         <v>35</v>
       </c>
       <c r="C138" s="19" t="s">
-        <v>242</v>
+        <v>250</v>
       </c>
     </row>
     <row r="139" spans="1:8" s="26" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A139" s="25" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="B139" s="29" t="s">
         <v>35</v>
       </c>
       <c r="C139" s="19" t="s">
-        <v>244</v>
+        <v>251</v>
       </c>
     </row>
     <row r="140" spans="1:8" s="26" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A140" s="25" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="B140" s="29" t="s">
         <v>35</v>
       </c>
       <c r="C140" s="19" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
     </row>
     <row r="141" spans="1:8" s="26" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A141" s="25" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="B141" s="29" t="s">
         <v>35</v>
       </c>
       <c r="C141" s="19" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
     </row>
     <row r="142" spans="1:8" s="26" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A142" s="25" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="B142" s="29" t="s">
         <v>35</v>
       </c>
       <c r="C142" s="19" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
     </row>
     <row r="143" spans="1:8" s="26" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A143" s="25" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="B143" s="29" t="s">
         <v>35</v>
       </c>
       <c r="C143" s="19" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
     </row>
     <row r="144" spans="1:8" s="26" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2615,7 +2625,7 @@
     </row>
     <row r="171" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A171" s="25" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="B171" s="29" t="s">
         <v>35</v>
@@ -2628,7 +2638,7 @@
         <v>0</v>
       </c>
       <c r="F171" s="5">
-        <v>110000</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="172" spans="1:8" s="26" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2911,7 +2921,7 @@
         <v>0</v>
       </c>
       <c r="F206" s="5">
-        <v>1</v>
+        <v>1499</v>
       </c>
       <c r="H206" s="1" t="s">
         <v>146</v>
@@ -2926,7 +2936,7 @@
         <v>0</v>
       </c>
       <c r="F207" s="5">
-        <v>400</v>
+        <v>1500</v>
       </c>
       <c r="H207" s="1" t="s">
         <v>147</v>
@@ -3060,10 +3070,10 @@
         <v>212</v>
       </c>
       <c r="F227" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G227" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="228" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3467,7 +3477,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="247" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B247" s="6" t="s">
         <v>15</v>
       </c>
@@ -3487,107 +3497,107 @@
         <v>0</v>
       </c>
     </row>
-    <row r="248" spans="1:8" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:8" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A248" s="25"/>
       <c r="C248" s="27"/>
     </row>
-    <row r="249" spans="1:8" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:8" s="26" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A249" s="25"/>
       <c r="C249" s="27"/>
     </row>
-    <row r="250" spans="1:8" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:8" s="26" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A250" s="25"/>
       <c r="C250" s="27"/>
     </row>
-    <row r="251" spans="1:8" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:8" s="26" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A251" s="25"/>
       <c r="C251" s="27"/>
     </row>
-    <row r="252" spans="1:8" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:8" s="26" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A252" s="25"/>
       <c r="C252" s="27"/>
     </row>
-    <row r="253" spans="1:8" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:8" s="26" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A253" s="25"/>
       <c r="C253" s="27"/>
     </row>
-    <row r="254" spans="1:8" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:8" s="26" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A254" s="25"/>
       <c r="C254" s="27"/>
     </row>
-    <row r="255" spans="1:8" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:8" s="26" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A255" s="25"/>
       <c r="C255" s="27"/>
     </row>
-    <row r="256" spans="1:8" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:8" s="26" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A256" s="25"/>
       <c r="C256" s="27"/>
     </row>
-    <row r="257" spans="1:3" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:3" s="26" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A257" s="25"/>
       <c r="C257" s="27"/>
     </row>
-    <row r="258" spans="1:3" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:3" s="26" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A258" s="25"/>
       <c r="C258" s="27"/>
     </row>
-    <row r="259" spans="1:3" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:3" s="26" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A259" s="25"/>
       <c r="C259" s="27"/>
     </row>
-    <row r="260" spans="1:3" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:3" s="26" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A260" s="25"/>
       <c r="C260" s="27"/>
     </row>
-    <row r="261" spans="1:3" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:3" s="26" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A261" s="25"/>
       <c r="C261" s="27"/>
     </row>
-    <row r="262" spans="1:3" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:3" s="26" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A262" s="25"/>
       <c r="C262" s="27"/>
     </row>
-    <row r="263" spans="1:3" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:3" s="26" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A263" s="25"/>
       <c r="C263" s="27"/>
     </row>
-    <row r="264" spans="1:3" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:3" s="26" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A264" s="25"/>
       <c r="C264" s="27"/>
     </row>
-    <row r="265" spans="1:3" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:3" s="26" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A265" s="25"/>
       <c r="C265" s="27"/>
     </row>
-    <row r="266" spans="1:3" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:3" s="26" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A266" s="25"/>
       <c r="C266" s="27"/>
     </row>
-    <row r="267" spans="1:3" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:3" s="26" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A267" s="25"/>
       <c r="C267" s="27"/>
     </row>
-    <row r="268" spans="1:3" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:3" s="26" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A268" s="25"/>
       <c r="C268" s="27"/>
     </row>
-    <row r="269" spans="1:3" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:3" s="26" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A269" s="25"/>
       <c r="C269" s="27"/>
     </row>
-    <row r="270" spans="1:3" s="26" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:3" s="26" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A270" s="25"/>
       <c r="C270" s="27"/>
     </row>
-    <row r="271" spans="1:3" s="26" customFormat="1" ht="11.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:3" s="26" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A271" s="25"/>
       <c r="C271" s="27"/>
     </row>
-    <row r="272" spans="1:3" s="26" customFormat="1" ht="11.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:3" s="26" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A272" s="25"/>
       <c r="C272" s="27"/>
     </row>
-    <row r="273" spans="1:8" ht="13.9" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="273" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="274" spans="1:8" s="38" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A274" s="35" t="s">
         <v>72</v>
@@ -3608,7 +3618,7 @@
         <v>75</v>
       </c>
       <c r="C275" s="5">
-        <v>0.12</v>
+        <v>0.16</v>
       </c>
     </row>
     <row r="276" spans="1:8" x14ac:dyDescent="0.25">
@@ -3650,12 +3660,25 @@
         <v>1</v>
       </c>
     </row>
-    <row r="279" spans="1:8" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="284" spans="1:8" ht="0.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="285" spans="1:8" ht="3.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="286" spans="1:8" ht="0.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="287" spans="1:8" ht="1.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="288" spans="1:8" ht="0.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="279" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="280" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="281" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="282" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="283" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="284" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="285" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="286" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="287" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="288" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="289" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="290" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="291" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="292" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="293" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="294" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="295" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="296" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="297" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
     <row r="298" spans="1:8" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A298" s="35" t="s">
         <v>169</v>
@@ -4012,38 +4035,38 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F322 C306:C321">
-    <cfRule type="containsText" dxfId="9" priority="7" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="1" priority="7" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",C306)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="8" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="0" priority="8" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",C306)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C300:C303">
-    <cfRule type="containsText" dxfId="7" priority="5" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="9" priority="5" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",C300)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="6" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="8" priority="6" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",C300)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F306:F312">
-    <cfRule type="containsText" dxfId="5" priority="3" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="7" priority="3" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",F306)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="4" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="6" priority="4" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",F306)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F313:F321">
-    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="5" priority="1" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",F313)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",F313)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations disablePrompts="1" xWindow="547" yWindow="733" count="35">
+  <dataValidations xWindow="547" yWindow="733" count="35">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Path the simulation directory" prompt="All inputs are saved in the so-called simulation directory, which includes, excel , gdx and pickle files together with the GAMS files._x000a__x000a_The path should be relative to this excel file. Use &quot;..&quot; to go up one folder. Folder separator can be either &quot;/&quot; or &quot;\&quot;" sqref="C34:D34" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
     <dataValidation type="date" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Start day of the simulation" prompt="This is the simulated day. It must be comprised within the range of dates provided within the data files." sqref="C57" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>1</formula1>
@@ -4096,7 +4119,7 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" xWindow="547" yWindow="733" count="9">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xWindow="547" yWindow="733" count="9">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000011000000}">
           <x14:formula1>
             <xm:f>Lists!$A$2:$A$3</xm:f>
@@ -5039,10 +5062,10 @@
     <sortCondition ref="D1"/>
   </sortState>
   <conditionalFormatting sqref="B2:O16">
-    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",B2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",B2)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
feat(gams): Boundary sector flexible supply (similar to flexible demand).
This makes both demand and supply flexible. Interesting for cases with limited resource availability. I.e. biomass etc. This is quantity based approach.
</commit_message>
<xml_diff>
--- a/ConfigFiles/ConfigTestBoundarySector.xlsx
+++ b/ConfigFiles/ConfigTestBoundarySector.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\Github\Dispa-SET.git\ConfigFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C86B7E1-7C14-4508-A54F-14C6CE94E675}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDDE4AC0-4BA7-43C9-B675-5F96A1E02C1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -779,9 +779,6 @@
     <t>Boundary Sector Demand (flexible)</t>
   </si>
   <si>
-    <t>Boundary Sector Capacity (flexible)</t>
-  </si>
-  <si>
     <t>GeoData (geographical coordinates)</t>
   </si>
   <si>
@@ -797,9 +794,6 @@
     <t>tests/dummy_data/boundary_sector/BS_FlexibleDemand.csv</t>
   </si>
   <si>
-    <t>tests/dummy_data/boundary_sector/BS_FlexibleCapacities.csv</t>
-  </si>
-  <si>
     <t>tests/dummy_data/boundary_sector/BS_Units_testcase.csv</t>
   </si>
   <si>
@@ -807,6 +801,12 @@
   </si>
   <si>
     <t>tests/dummy_data/HeatDemand.csv</t>
+  </si>
+  <si>
+    <t>Boundary Sector Supply (flexible)</t>
+  </si>
+  <si>
+    <t>tests/dummy_data/boundary_sector/BS_FlexibleSupply.csv</t>
   </si>
 </sst>
 </file>
@@ -1566,7 +1566,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:H330"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A237" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A227" workbookViewId="0">
       <selection activeCell="C276" sqref="C276"/>
     </sheetView>
   </sheetViews>
@@ -2199,7 +2199,7 @@
         <v>35</v>
       </c>
       <c r="C128" s="19" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="D128" s="18" t="s">
         <v>87</v>
@@ -2310,7 +2310,7 @@
         <v>35</v>
       </c>
       <c r="C135" s="19" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D135" s="18" t="s">
         <v>87</v>
@@ -2324,7 +2324,7 @@
         <v>35</v>
       </c>
       <c r="C136" s="19" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="D136" s="18" t="s">
         <v>87</v>
@@ -2333,7 +2333,7 @@
     </row>
     <row r="137" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A137" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B137" s="29" t="s">
         <v>35</v>
@@ -2353,7 +2353,7 @@
         <v>35</v>
       </c>
       <c r="C138" s="19" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="139" spans="1:8" s="26" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2364,7 +2364,7 @@
         <v>35</v>
       </c>
       <c r="C139" s="19" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="140" spans="1:8" s="26" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2397,18 +2397,18 @@
         <v>35</v>
       </c>
       <c r="C142" s="19" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="143" spans="1:8" s="26" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A143" s="25" t="s">
-        <v>247</v>
+        <v>255</v>
       </c>
       <c r="B143" s="29" t="s">
         <v>35</v>
       </c>
       <c r="C143" s="19" t="s">
-        <v>253</v>
+        <v>256</v>
       </c>
     </row>
     <row r="144" spans="1:8" s="26" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2625,7 +2625,7 @@
     </row>
     <row r="171" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A171" s="25" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B171" s="29" t="s">
         <v>35</v>
@@ -4035,34 +4035,34 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F322 C306:C321">
-    <cfRule type="containsText" dxfId="1" priority="7" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="9" priority="7" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",C306)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="8" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="8" priority="8" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",C306)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C300:C303">
-    <cfRule type="containsText" dxfId="9" priority="5" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="7" priority="5" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",C300)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="6" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="6" priority="6" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",C300)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F306:F312">
-    <cfRule type="containsText" dxfId="7" priority="3" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="5" priority="3" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",F306)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="4" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="4" priority="4" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",F306)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F313:F321">
-    <cfRule type="containsText" dxfId="5" priority="1" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",F313)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",F313)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5062,10 +5062,10 @@
     <sortCondition ref="D1"/>
   </sortState>
   <conditionalFormatting sqref="B2:O16">
-    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",B2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",B2)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
feat(boundary_sector): spillage between boundary sector zones (good for hydro cascade systems)
New inputs: ConfigFile Maximum allowed spillage

New results: LostLoad_BoundarySectorSpillage, OutputBoundarySectorSpillage
</commit_message>
<xml_diff>
--- a/ConfigFiles/ConfigTestBoundarySector.xlsx
+++ b/ConfigFiles/ConfigTestBoundarySector.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\Github\Dispa-SET.git\ConfigFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5311CF67-67A2-4894-A9C5-2F68E1A863AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E60EE28-991B-4D12-B96E-0E605A9FDF29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="261">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="263">
   <si>
     <t>Default value</t>
   </si>
@@ -819,6 +819,12 @@
   </si>
   <si>
     <t>Default</t>
+  </si>
+  <si>
+    <t>Boundary Sector Max Spillage</t>
+  </si>
+  <si>
+    <t>tests/dummy_data/boundary_sector/BS_Spillage_Capacity.csv</t>
   </si>
 </sst>
 </file>
@@ -1099,6 +1105,9 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="10" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1113,9 +1122,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1566,8 +1572,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:H330"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A206" workbookViewId="0">
-      <selection activeCell="A146" sqref="A146"/>
+    <sheetView tabSelected="1" topLeftCell="A99" workbookViewId="0">
+      <selection activeCell="C145" sqref="C145"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1584,16 +1590,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="44" t="s">
         <v>239</v>
       </c>
-      <c r="B1" s="43"/>
-      <c r="C1" s="43"/>
-      <c r="D1" s="43"/>
-      <c r="E1" s="43"/>
-      <c r="F1" s="43"/>
-      <c r="G1" s="43"/>
-      <c r="H1" s="43"/>
+      <c r="B1" s="44"/>
+      <c r="C1" s="44"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
+      <c r="G1" s="44"/>
+      <c r="H1" s="44"/>
     </row>
     <row r="2" spans="1:8" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
@@ -1608,15 +1614,15 @@
     <row r="3" spans="1:8" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="1:8" s="31" customFormat="1" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="30"/>
-      <c r="B4" s="44" t="s">
+      <c r="B4" s="45" t="s">
         <v>56</v>
       </c>
-      <c r="C4" s="44"/>
-      <c r="D4" s="44"/>
-      <c r="E4" s="44"/>
-      <c r="F4" s="44"/>
-      <c r="G4" s="44"/>
-      <c r="H4" s="44"/>
+      <c r="C4" s="45"/>
+      <c r="D4" s="45"/>
+      <c r="E4" s="45"/>
+      <c r="F4" s="45"/>
+      <c r="G4" s="45"/>
+      <c r="H4" s="45"/>
     </row>
     <row r="5" spans="1:8" s="8" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="7"/>
@@ -1632,15 +1638,15 @@
       <c r="A6" s="36" t="s">
         <v>49</v>
       </c>
-      <c r="B6" s="41" t="s">
+      <c r="B6" s="42" t="s">
         <v>181</v>
       </c>
-      <c r="C6" s="41"/>
-      <c r="D6" s="41"/>
-      <c r="E6" s="41"/>
-      <c r="F6" s="41"/>
-      <c r="G6" s="41"/>
-      <c r="H6" s="41"/>
+      <c r="C6" s="42"/>
+      <c r="D6" s="42"/>
+      <c r="E6" s="42"/>
+      <c r="F6" s="42"/>
+      <c r="G6" s="42"/>
+      <c r="H6" s="42"/>
     </row>
     <row r="7" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="12"/>
@@ -1841,7 +1847,7 @@
       <c r="B39" s="25" t="s">
         <v>258</v>
       </c>
-      <c r="C39" s="46">
+      <c r="C39" s="41">
         <v>5.9999999999999995E-4</v>
       </c>
     </row>
@@ -2432,7 +2438,15 @@
       </c>
     </row>
     <row r="144" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C144" s="40"/>
+      <c r="A144" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="B144" s="26" t="s">
+        <v>35</v>
+      </c>
+      <c r="C144" s="19" t="s">
+        <v>262</v>
+      </c>
     </row>
     <row r="145" spans="3:3" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C145" s="40"/>
@@ -2921,7 +2935,7 @@
       </c>
     </row>
     <row r="227" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A227" s="42" t="s">
+      <c r="A227" s="43" t="s">
         <v>51</v>
       </c>
       <c r="B227" s="6" t="s">
@@ -2944,7 +2958,7 @@
       </c>
     </row>
     <row r="228" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A228" s="42"/>
+      <c r="A228" s="43"/>
       <c r="B228" s="6" t="s">
         <v>21</v>
       </c>
@@ -2965,7 +2979,7 @@
       </c>
     </row>
     <row r="229" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A229" s="42"/>
+      <c r="A229" s="43"/>
       <c r="B229" s="6" t="s">
         <v>149</v>
       </c>
@@ -2986,7 +3000,7 @@
       </c>
     </row>
     <row r="230" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A230" s="42"/>
+      <c r="A230" s="43"/>
       <c r="B230" s="6" t="s">
         <v>131</v>
       </c>
@@ -3007,7 +3021,7 @@
       </c>
     </row>
     <row r="231" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A231" s="42"/>
+      <c r="A231" s="43"/>
       <c r="B231" s="6" t="s">
         <v>5</v>
       </c>
@@ -3028,7 +3042,7 @@
       </c>
     </row>
     <row r="232" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A232" s="42"/>
+      <c r="A232" s="43"/>
       <c r="B232" s="6" t="s">
         <v>152</v>
       </c>
@@ -3049,7 +3063,7 @@
       </c>
     </row>
     <row r="233" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A233" s="42"/>
+      <c r="A233" s="43"/>
       <c r="B233" s="6" t="s">
         <v>30</v>
       </c>
@@ -3070,7 +3084,7 @@
       </c>
     </row>
     <row r="234" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A234" s="42"/>
+      <c r="A234" s="43"/>
       <c r="B234" s="6" t="s">
         <v>16</v>
       </c>
@@ -3091,7 +3105,7 @@
       </c>
     </row>
     <row r="235" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A235" s="42"/>
+      <c r="A235" s="43"/>
       <c r="B235" s="6" t="s">
         <v>6</v>
       </c>
@@ -3112,7 +3126,7 @@
       </c>
     </row>
     <row r="236" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A236" s="42"/>
+      <c r="A236" s="43"/>
       <c r="B236" s="6" t="s">
         <v>8</v>
       </c>
@@ -3133,7 +3147,7 @@
       </c>
     </row>
     <row r="237" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A237" s="42"/>
+      <c r="A237" s="43"/>
       <c r="B237" s="6" t="s">
         <v>7</v>
       </c>
@@ -3154,7 +3168,7 @@
       </c>
     </row>
     <row r="238" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A238" s="42"/>
+      <c r="A238" s="43"/>
       <c r="B238" s="6" t="s">
         <v>9</v>
       </c>
@@ -3175,7 +3189,7 @@
       </c>
     </row>
     <row r="239" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A239" s="42"/>
+      <c r="A239" s="43"/>
       <c r="B239" s="6" t="s">
         <v>11</v>
       </c>
@@ -3196,7 +3210,7 @@
       </c>
     </row>
     <row r="240" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A240" s="42"/>
+      <c r="A240" s="43"/>
       <c r="B240" s="6" t="s">
         <v>12</v>
       </c>
@@ -3217,7 +3231,7 @@
       </c>
     </row>
     <row r="241" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A241" s="42"/>
+      <c r="A241" s="43"/>
       <c r="B241" s="6" t="s">
         <v>27</v>
       </c>
@@ -3298,7 +3312,7 @@
       </c>
     </row>
     <row r="245" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A245" s="45" t="s">
+      <c r="A245" s="46" t="s">
         <v>170</v>
       </c>
       <c r="B245" s="6" t="s">
@@ -3321,7 +3335,7 @@
       </c>
     </row>
     <row r="246" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A246" s="45"/>
+      <c r="A246" s="46"/>
       <c r="B246" s="6" t="s">
         <v>158</v>
       </c>

</xml_diff>

<commit_message>
feat(heat): improved representation of heating technologies in Sector X
</commit_message>
<xml_diff>
--- a/ConfigFiles/ConfigTestBoundarySector.xlsx
+++ b/ConfigFiles/ConfigTestBoundarySector.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25726"/>
   <workbookPr updateLinks="never" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\Github\Dispa-SET.git\ConfigFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E60EE28-991B-4D12-B96E-0E605A9FDF29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AD00CC7-93AD-4D1D-887B-3C6619463C35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="263">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="262">
   <si>
     <t>Default value</t>
   </si>
@@ -425,9 +425,6 @@
     <t>CPLEX path</t>
   </si>
   <si>
-    <t>Heat Demand</t>
-  </si>
-  <si>
     <t>Integer clustering</t>
   </si>
   <si>
@@ -800,9 +797,6 @@
     <t>tests/dummy_data/Temperatures.csv</t>
   </si>
   <si>
-    <t>tests/dummy_data/HeatDemand.csv</t>
-  </si>
-  <si>
     <t>Boundary Sector Supply (flexible)</t>
   </si>
   <si>
@@ -825,6 +819,9 @@
   </si>
   <si>
     <t>tests/dummy_data/boundary_sector/BS_Spillage_Capacity.csv</t>
+  </si>
+  <si>
+    <t>Scaled outflows</t>
   </si>
 </sst>
 </file>
@@ -1573,7 +1570,7 @@
   <dimension ref="A1:H330"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A99" workbookViewId="0">
-      <selection activeCell="C145" sqref="C145"/>
+      <selection activeCell="A135" sqref="A135"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1591,7 +1588,7 @@
   <sheetData>
     <row r="1" spans="1:8" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="44" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B1" s="44"/>
       <c r="C1" s="44"/>
@@ -1639,7 +1636,7 @@
         <v>49</v>
       </c>
       <c r="B6" s="42" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C6" s="42"/>
       <c r="D6" s="42"/>
@@ -1722,7 +1719,7 @@
     </row>
     <row r="15" spans="1:8" s="35" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="32" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B15" s="33"/>
       <c r="C15" s="34"/>
@@ -1740,13 +1737,13 @@
     </row>
     <row r="17" spans="1:2" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B17" s="27"/>
     </row>
     <row r="18" spans="1:2" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B18" s="25"/>
     </row>
@@ -1766,7 +1763,7 @@
     <row r="32" spans="1:2" ht="9.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="33" spans="1:8" s="35" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="32" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B33" s="33"/>
       <c r="C33" s="34"/>
@@ -1784,7 +1781,7 @@
         <v>35</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D34" s="13"/>
       <c r="H34" s="1" t="s">
@@ -1842,10 +1839,10 @@
     </row>
     <row r="39" spans="1:8" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="B39" s="25" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="C39" s="41">
         <v>5.9999999999999995E-4</v>
@@ -1853,13 +1850,13 @@
     </row>
     <row r="40" spans="1:8" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F40" s="2" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="G40" s="27" t="s">
         <v>59</v>
       </c>
       <c r="H40" s="4" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="41" spans="1:8" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1879,7 +1876,7 @@
     <row r="55" spans="1:8" ht="13.9" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="56" spans="1:8" s="35" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="32" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B56" s="33"/>
       <c r="C56" s="34"/>
@@ -1944,10 +1941,10 @@
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B61" s="25" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C61" s="4">
         <v>1</v>
@@ -1955,10 +1952,10 @@
     </row>
     <row r="62" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="B62" s="25" t="s">
         <v>200</v>
-      </c>
-      <c r="B62" s="25" t="s">
-        <v>201</v>
       </c>
       <c r="C62" s="4">
         <v>1</v>
@@ -1978,7 +1975,7 @@
     <row r="74" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="75" spans="1:8" s="35" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="32" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B75" s="33"/>
       <c r="C75" s="34"/>
@@ -1999,7 +1996,7 @@
         <v>59</v>
       </c>
       <c r="C77" s="4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H77" s="1" t="s">
         <v>63</v>
@@ -2013,7 +2010,7 @@
         <v>59</v>
       </c>
       <c r="C78" s="4" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="H78" s="1" t="s">
         <v>64</v>
@@ -2056,7 +2053,7 @@
     <row r="97" spans="1:8" ht="13.9" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="98" spans="1:8" s="35" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="32" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B98" s="33"/>
       <c r="C98" s="34"/>
@@ -2068,35 +2065,35 @@
     </row>
     <row r="99" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B99" s="27" t="s">
         <v>59</v>
       </c>
       <c r="C99" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="H99" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B100" s="27" t="s">
         <v>59</v>
       </c>
       <c r="C100" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="H100" s="1" t="s">
         <v>162</v>
-      </c>
-      <c r="H100" s="1" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="101" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B101" s="27" t="s">
         <v>4</v>
@@ -2107,7 +2104,7 @@
     </row>
     <row r="102" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" s="29" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E102" s="25" t="s">
         <v>0</v>
@@ -2116,12 +2113,12 @@
         <v>0.5</v>
       </c>
       <c r="H102" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="103" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" s="29" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E103" s="25" t="s">
         <v>0</v>
@@ -2130,7 +2127,7 @@
         <v>0.5</v>
       </c>
       <c r="H103" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="104" spans="1:8" ht="9" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2158,7 +2155,7 @@
     </row>
     <row r="124" spans="1:8" s="35" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A124" s="32" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B124" s="33"/>
       <c r="C124" s="34"/>
@@ -2176,7 +2173,7 @@
         <v>35</v>
       </c>
       <c r="C125" s="19" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D125" s="18" t="s">
         <v>87</v>
@@ -2185,7 +2182,7 @@
     </row>
     <row r="126" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A126" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B126" s="26" t="s">
         <v>35</v>
@@ -2225,13 +2222,13 @@
         <v>35</v>
       </c>
       <c r="C128" s="19" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D128" s="18" t="s">
         <v>87</v>
       </c>
       <c r="H128" s="11" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="129" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2242,7 +2239,7 @@
         <v>35</v>
       </c>
       <c r="C129" s="19" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D129" s="18" t="s">
         <v>87</v>
@@ -2277,7 +2274,7 @@
         <v>35</v>
       </c>
       <c r="C131" s="19" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D131" s="18" t="s">
         <v>87</v>
@@ -2330,27 +2327,25 @@
     </row>
     <row r="135" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A135" s="2" t="s">
-        <v>129</v>
+        <v>261</v>
       </c>
       <c r="B135" s="26" t="s">
         <v>35</v>
       </c>
-      <c r="C135" s="19" t="s">
-        <v>254</v>
-      </c>
+      <c r="C135" s="19"/>
       <c r="D135" s="18" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="136" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A136" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B136" s="26" t="s">
         <v>35</v>
       </c>
       <c r="C136" s="19" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D136" s="18" t="s">
         <v>87</v>
@@ -2359,13 +2354,13 @@
     </row>
     <row r="137" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A137" s="2" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B137" s="26" t="s">
         <v>35</v>
       </c>
       <c r="C137" s="19" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D137" s="18" t="s">
         <v>87</v>
@@ -2373,79 +2368,79 @@
     </row>
     <row r="138" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A138" s="2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B138" s="26" t="s">
         <v>35</v>
       </c>
       <c r="C138" s="19" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="139" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A139" s="2" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B139" s="26" t="s">
         <v>35</v>
       </c>
       <c r="C139" s="19" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="140" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A140" s="2" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B140" s="26" t="s">
         <v>35</v>
       </c>
       <c r="C140" s="19" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="141" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A141" s="2" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B141" s="26" t="s">
         <v>35</v>
       </c>
       <c r="C141" s="19" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="142" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A142" s="2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B142" s="26" t="s">
         <v>35</v>
       </c>
       <c r="C142" s="19" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="143" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A143" s="2" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="B143" s="26" t="s">
         <v>35</v>
       </c>
       <c r="C143" s="19" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="144" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A144" s="2" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="B144" s="26" t="s">
         <v>35</v>
       </c>
       <c r="C144" s="19" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="145" spans="3:3" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2470,7 +2465,7 @@
     <row r="160" spans="3:3" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="161" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A161" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B161" s="26" t="s">
         <v>35</v>
@@ -2479,7 +2474,7 @@
     </row>
     <row r="162" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A162" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B162" s="26" t="s">
         <v>35</v>
@@ -2488,7 +2483,7 @@
     </row>
     <row r="163" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A163" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C163" s="1"/>
       <c r="E163" s="25" t="s">
@@ -2498,12 +2493,12 @@
         <v>4</v>
       </c>
       <c r="H163" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="164" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A164" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E164" s="25" t="s">
         <v>0</v>
@@ -2512,13 +2507,13 @@
         <v>0.5</v>
       </c>
       <c r="H164" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="165" spans="1:8" ht="13.9" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="166" spans="1:8" s="35" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A166" s="32" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B166" s="33"/>
       <c r="C166" s="34"/>
@@ -2548,7 +2543,7 @@
     </row>
     <row r="168" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A168" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B168" s="26" t="s">
         <v>35</v>
@@ -2566,7 +2561,7 @@
     </row>
     <row r="169" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A169" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B169" s="26" t="s">
         <v>35</v>
@@ -2582,12 +2577,12 @@
         <v>400</v>
       </c>
       <c r="H169" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="170" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A170" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B170" s="26" t="s">
         <v>35</v>
@@ -2603,12 +2598,12 @@
         <v>0</v>
       </c>
       <c r="H170" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="171" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A171" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B171" s="26" t="s">
         <v>35</v>
@@ -2626,7 +2621,7 @@
     </row>
     <row r="172" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A172" s="2" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B172" s="26" t="s">
         <v>35</v>
@@ -2677,7 +2672,7 @@
         <v>35</v>
       </c>
       <c r="C182" s="19" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D182" s="18" t="s">
         <v>87</v>
@@ -2697,7 +2692,7 @@
         <v>35</v>
       </c>
       <c r="C183" s="19" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D183" s="18" t="s">
         <v>87</v>
@@ -2720,7 +2715,7 @@
         <v>35</v>
       </c>
       <c r="C184" s="19" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D184" s="18" t="s">
         <v>87</v>
@@ -2740,7 +2735,7 @@
         <v>35</v>
       </c>
       <c r="C185" s="19" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D185" s="18" t="s">
         <v>87</v>
@@ -2778,7 +2773,7 @@
         <v>35</v>
       </c>
       <c r="C187" s="19" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D187" s="18" t="s">
         <v>87</v>
@@ -2792,7 +2787,7 @@
     </row>
     <row r="188" spans="1:8" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A188" s="2" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B188" s="26" t="s">
         <v>35</v>
@@ -2825,7 +2820,7 @@
     <row r="204" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="205" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A205" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C205" s="1"/>
       <c r="E205" s="25" t="s">
@@ -2835,12 +2830,12 @@
         <v>100000</v>
       </c>
       <c r="H205" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="206" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A206" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C206" s="1"/>
       <c r="E206" s="25" t="s">
@@ -2850,12 +2845,12 @@
         <v>1499</v>
       </c>
       <c r="H206" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="207" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A207" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C207" s="1"/>
       <c r="E207" s="25" t="s">
@@ -2865,7 +2860,7 @@
         <v>1500</v>
       </c>
       <c r="H207" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="209" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2889,25 +2884,25 @@
     </row>
     <row r="225" spans="1:8" s="38" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A225" s="36" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B225" s="28" t="s">
         <v>4</v>
       </c>
       <c r="C225" s="36" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D225" s="39" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E225" s="28" t="s">
         <v>4</v>
       </c>
       <c r="F225" s="36" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="G225" s="36" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="H225" s="37"/>
     </row>
@@ -2916,7 +2911,7 @@
         <v>50</v>
       </c>
       <c r="B226" s="6" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C226" s="4" t="b">
         <v>0</v>
@@ -2925,7 +2920,7 @@
         <v>0</v>
       </c>
       <c r="E226" s="6" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F226" s="4" t="b">
         <v>1</v>
@@ -2939,7 +2934,7 @@
         <v>51</v>
       </c>
       <c r="B227" s="6" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C227" s="4" t="b">
         <v>1</v>
@@ -2948,7 +2943,7 @@
         <v>1</v>
       </c>
       <c r="E227" s="6" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F227" s="4" t="b">
         <v>1</v>
@@ -2981,7 +2976,7 @@
     <row r="229" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A229" s="43"/>
       <c r="B229" s="6" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C229" s="4" t="b">
         <v>0</v>
@@ -3002,7 +2997,7 @@
     <row r="230" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A230" s="43"/>
       <c r="B230" s="6" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C230" s="4" t="b">
         <v>0</v>
@@ -3011,7 +3006,7 @@
         <v>0</v>
       </c>
       <c r="E230" s="6" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F230" s="4" t="b">
         <v>0</v>
@@ -3032,7 +3027,7 @@
         <v>0</v>
       </c>
       <c r="E231" s="6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F231" s="4" t="b">
         <v>0</v>
@@ -3044,16 +3039,16 @@
     <row r="232" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A232" s="43"/>
       <c r="B232" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="C232" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="D232" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="E232" s="6" t="s">
         <v>152</v>
-      </c>
-      <c r="C232" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="D232" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="E232" s="6" t="s">
-        <v>153</v>
       </c>
       <c r="F232" s="4" t="b">
         <v>0</v>
@@ -3095,7 +3090,7 @@
         <v>0</v>
       </c>
       <c r="E234" s="6" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F234" s="4" t="b">
         <v>0</v>
@@ -3200,7 +3195,7 @@
         <v>0</v>
       </c>
       <c r="E239" s="6" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F239" s="4" t="b">
         <v>0</v>
@@ -3221,7 +3216,7 @@
         <v>0</v>
       </c>
       <c r="E240" s="6" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F240" s="4" t="b">
         <v>0</v>
@@ -3302,7 +3297,7 @@
         <v>0</v>
       </c>
       <c r="E244" s="6" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F244" s="4" t="b">
         <v>0</v>
@@ -3313,7 +3308,7 @@
     </row>
     <row r="245" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A245" s="46" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B245" s="6" t="s">
         <v>10</v>
@@ -3325,7 +3320,7 @@
         <v>0</v>
       </c>
       <c r="E245" s="6" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F245" s="4" t="b">
         <v>0</v>
@@ -3337,7 +3332,7 @@
     <row r="246" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A246" s="46"/>
       <c r="B246" s="6" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C246" s="4" t="b">
         <v>0</v>
@@ -3355,7 +3350,7 @@
         <v>0</v>
       </c>
       <c r="H246" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="247" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3369,7 +3364,7 @@
         <v>0</v>
       </c>
       <c r="E247" s="6" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F247" s="4" t="b">
         <v>0</v>
@@ -3487,7 +3482,7 @@
     <row r="297" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
     <row r="298" spans="1:8" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A298" s="32" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B298" s="33"/>
       <c r="C298" s="34"/>
@@ -3499,7 +3494,7 @@
     </row>
     <row r="299" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A299" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C299" s="28" t="s">
         <v>4</v>
@@ -3554,7 +3549,7 @@
     </row>
     <row r="305" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A305" s="2" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C305" s="28" t="s">
         <v>4</v>
@@ -3571,7 +3566,7 @@
         <v>1</v>
       </c>
       <c r="E306" s="22" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="F306" s="21" t="b">
         <v>1</v>
@@ -3585,7 +3580,7 @@
         <v>1</v>
       </c>
       <c r="E307" s="22" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="F307" s="21" t="b">
         <v>1</v>
@@ -3599,7 +3594,7 @@
         <v>1</v>
       </c>
       <c r="E308" s="22" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="F308" s="21" t="b">
         <v>1</v>
@@ -3613,7 +3608,7 @@
         <v>0</v>
       </c>
       <c r="E309" s="22" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F309" s="21" t="b">
         <v>1</v>
@@ -3627,7 +3622,7 @@
         <v>1</v>
       </c>
       <c r="E310" s="22" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F310" s="21" t="b">
         <v>1</v>
@@ -3641,7 +3636,7 @@
         <v>1</v>
       </c>
       <c r="E311" s="22" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="F311" s="21" t="b">
         <v>1</v>
@@ -3655,7 +3650,7 @@
         <v>0</v>
       </c>
       <c r="E312" s="22" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="F312" s="21" t="b">
         <v>1</v>
@@ -3669,7 +3664,7 @@
         <v>0</v>
       </c>
       <c r="E313" s="22" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F313" s="21" t="b">
         <v>0</v>
@@ -3683,7 +3678,7 @@
         <v>0</v>
       </c>
       <c r="E314" s="22" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F314" s="21" t="b">
         <v>0</v>
@@ -3697,7 +3692,7 @@
         <v>0</v>
       </c>
       <c r="E315" s="22" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F315" s="21" t="b">
         <v>0</v>
@@ -3711,7 +3706,7 @@
         <v>1</v>
       </c>
       <c r="E316" s="22" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F316" s="21" t="b">
         <v>0</v>
@@ -3725,7 +3720,7 @@
         <v>1</v>
       </c>
       <c r="E317" s="22" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="F317" s="21" t="b">
         <v>0</v>
@@ -3739,7 +3734,7 @@
         <v>1</v>
       </c>
       <c r="E318" s="22" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="F318" s="21" t="b">
         <v>0</v>
@@ -3753,7 +3748,7 @@
         <v>0</v>
       </c>
       <c r="E319" s="22" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="F319" s="21" t="b">
         <v>0</v>
@@ -3767,7 +3762,7 @@
         <v>0</v>
       </c>
       <c r="E320" s="22" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="F320" s="21" t="b">
         <v>0</v>
@@ -3775,13 +3770,13 @@
     </row>
     <row r="321" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B321" s="22" t="s">
+        <v>232</v>
+      </c>
+      <c r="C321" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="E321" s="22" t="s">
         <v>233</v>
-      </c>
-      <c r="C321" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="E321" s="22" t="s">
-        <v>234</v>
       </c>
       <c r="F321" s="21" t="b">
         <v>0</v>
@@ -3789,7 +3784,7 @@
     </row>
     <row r="322" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E322" s="22" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="F322" s="21" t="b">
         <v>0</v>
@@ -3797,7 +3792,7 @@
     </row>
     <row r="325" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A325" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="330" spans="1:6" x14ac:dyDescent="0.25">
@@ -4006,10 +4001,10 @@
         <v>79</v>
       </c>
       <c r="E1" s="16" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F1" s="16" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -4017,7 +4012,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C2" t="s">
         <v>58</v>
@@ -4026,10 +4021,10 @@
         <v>82</v>
       </c>
       <c r="E2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -4040,16 +4035,16 @@
         <v>43</v>
       </c>
       <c r="C3" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D3" t="s">
         <v>83</v>
       </c>
       <c r="E3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -4057,21 +4052,21 @@
         <v>44</v>
       </c>
       <c r="C4" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D4" t="s">
         <v>80</v>
       </c>
       <c r="E4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C5" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D5" t="s">
         <v>81</v>
@@ -4079,7 +4074,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat(MTS): introduced cycling storage conditions
</commit_message>
<xml_diff>
--- a/ConfigFiles/ConfigTestBoundarySector.xlsx
+++ b/ConfigFiles/ConfigTestBoundarySector.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\Github\Dispa-SET.git\ConfigFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AD00CC7-93AD-4D1D-887B-3C6619463C35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{740A5B4E-DE1D-4749-B35F-1833C2414B22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="262">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="263">
   <si>
     <t>Default value</t>
   </si>
@@ -822,6 +822,9 @@
   </si>
   <si>
     <t>Scaled outflows</t>
+  </si>
+  <si>
+    <t>Boundary Sector Reservoir Level</t>
   </si>
 </sst>
 </file>
@@ -1570,7 +1573,7 @@
   <dimension ref="A1:H330"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A99" workbookViewId="0">
-      <selection activeCell="A135" sqref="A135"/>
+      <selection activeCell="A145" sqref="A145"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2443,26 +2446,32 @@
         <v>260</v>
       </c>
     </row>
-    <row r="145" spans="3:3" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C145" s="40"/>
-    </row>
-    <row r="146" spans="3:3" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:3" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A145" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="B145" s="26" t="s">
+        <v>35</v>
+      </c>
+      <c r="C145" s="19"/>
+    </row>
+    <row r="146" spans="1:3" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C146" s="40"/>
     </row>
-    <row r="147" spans="3:3" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="148" spans="3:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="149" spans="3:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="150" spans="3:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="151" spans="3:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="152" spans="3:3" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="153" spans="3:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="154" spans="3:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="155" spans="3:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="156" spans="3:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="157" spans="3:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="158" spans="3:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="159" spans="3:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="160" spans="3:3" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="147" spans="1:3" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="148" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="149" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="150" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="151" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="152" spans="1:3" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="153" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="154" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="155" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="156" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="157" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="158" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="159" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="160" spans="1:3" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="161" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A161" s="2" t="s">
         <v>209</v>

</xml_diff>

<commit_message>
integrating DC power flow into the pre-processing (wip)
</commit_message>
<xml_diff>
--- a/ConfigFiles/ConfigTestBoundarySector.xlsx
+++ b/ConfigFiles/ConfigTestBoundarySector.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26227"/>
   <workbookPr updateLinks="never" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\Github\Dispa-SET.git\ConfigFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Sylvain\svn\Dispa-SET_Public\ConfigFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{740A5B4E-DE1D-4749-B35F-1833C2414B22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB8147E1-5B6B-4FCF-A118-06C55675D59E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="263">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="268">
   <si>
     <t>Default value</t>
   </si>
@@ -578,9 +578,6 @@
     <t>Active zone</t>
   </si>
   <si>
-    <t>Dummy configuration file for testing purposes. Two fictitious zones (Z1 and Z2) are simulated. The simulated period is only 7 days. There is a CHP unit in zone 1</t>
-  </si>
-  <si>
     <t>tests/dummy_data/Load_RealTime/##/2015.csv</t>
   </si>
   <si>
@@ -752,9 +749,6 @@
     <t>Simulations/simulation_test_bs</t>
   </si>
   <si>
-    <t>Dispa-SET Configuration File (v20.03)</t>
-  </si>
-  <si>
     <t>Boundary Sector Demand</t>
   </si>
   <si>
@@ -825,6 +819,27 @@
   </si>
   <si>
     <t>Boundary Sector Reservoir Level</t>
+  </si>
+  <si>
+    <t>Dispa-SET Configuration File (v23.04)</t>
+  </si>
+  <si>
+    <t>Dummy configuration file for testing purposes. Three fictitious zones (Z1,  Z2 and ZZ3) are simulated. The simulated period is only 7 days. There is a CHP unit in zone 1</t>
+  </si>
+  <si>
+    <t>Transmission grid type</t>
+  </si>
+  <si>
+    <t>Transmision grid type</t>
+  </si>
+  <si>
+    <t>DC-Power Flow</t>
+  </si>
+  <si>
+    <t>Grid Data</t>
+  </si>
+  <si>
+    <t>Only used if DC power flow is activated. The table provides the physical characteristics of each line</t>
   </si>
 </sst>
 </file>
@@ -985,7 +1000,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1101,9 +1116,6 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1249,7 +1261,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1572,11 +1584,11 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:H330"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A99" workbookViewId="0">
-      <selection activeCell="A145" sqref="A145"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H147" sqref="H147"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="48.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.42578125" style="1" customWidth="1"/>
@@ -1590,16 +1602,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="44" t="s">
-        <v>238</v>
-      </c>
-      <c r="B1" s="44"/>
-      <c r="C1" s="44"/>
-      <c r="D1" s="44"/>
-      <c r="E1" s="44"/>
-      <c r="F1" s="44"/>
-      <c r="G1" s="44"/>
-      <c r="H1" s="44"/>
+      <c r="A1" s="43" t="s">
+        <v>261</v>
+      </c>
+      <c r="B1" s="43"/>
+      <c r="C1" s="43"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="43"/>
+      <c r="G1" s="43"/>
+      <c r="H1" s="43"/>
     </row>
     <row r="2" spans="1:8" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
@@ -1614,15 +1626,15 @@
     <row r="3" spans="1:8" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="1:8" s="31" customFormat="1" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="30"/>
-      <c r="B4" s="45" t="s">
+      <c r="B4" s="44" t="s">
         <v>56</v>
       </c>
-      <c r="C4" s="45"/>
-      <c r="D4" s="45"/>
-      <c r="E4" s="45"/>
-      <c r="F4" s="45"/>
-      <c r="G4" s="45"/>
-      <c r="H4" s="45"/>
+      <c r="C4" s="44"/>
+      <c r="D4" s="44"/>
+      <c r="E4" s="44"/>
+      <c r="F4" s="44"/>
+      <c r="G4" s="44"/>
+      <c r="H4" s="44"/>
     </row>
     <row r="5" spans="1:8" s="8" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="7"/>
@@ -1638,15 +1650,15 @@
       <c r="A6" s="36" t="s">
         <v>49</v>
       </c>
-      <c r="B6" s="42" t="s">
-        <v>180</v>
-      </c>
-      <c r="C6" s="42"/>
-      <c r="D6" s="42"/>
-      <c r="E6" s="42"/>
-      <c r="F6" s="42"/>
-      <c r="G6" s="42"/>
-      <c r="H6" s="42"/>
+      <c r="B6" s="41" t="s">
+        <v>262</v>
+      </c>
+      <c r="C6" s="41"/>
+      <c r="D6" s="41"/>
+      <c r="E6" s="41"/>
+      <c r="F6" s="41"/>
+      <c r="G6" s="41"/>
+      <c r="H6" s="41"/>
     </row>
     <row r="7" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="12"/>
@@ -1784,7 +1796,7 @@
         <v>35</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D34" s="13"/>
       <c r="H34" s="1" t="s">
@@ -1842,24 +1854,24 @@
     </row>
     <row r="39" spans="1:8" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="B39" s="25" t="s">
+        <v>254</v>
+      </c>
+      <c r="C39" s="40">
+        <v>5.9999999999999995E-4</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="2" t="s">
         <v>255</v>
       </c>
-      <c r="B39" s="25" t="s">
+      <c r="B40" s="27" t="s">
+        <v>59</v>
+      </c>
+      <c r="C40" s="4" t="s">
         <v>256</v>
-      </c>
-      <c r="C39" s="41">
-        <v>5.9999999999999995E-4</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F40" s="2" t="s">
-        <v>257</v>
-      </c>
-      <c r="G40" s="27" t="s">
-        <v>59</v>
-      </c>
-      <c r="H40" s="4" t="s">
-        <v>258</v>
       </c>
     </row>
     <row r="41" spans="1:8" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1944,10 +1956,10 @@
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B61" s="25" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C61" s="4">
         <v>1</v>
@@ -1955,10 +1967,10 @@
     </row>
     <row r="62" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="B62" s="25" t="s">
         <v>199</v>
-      </c>
-      <c r="B62" s="25" t="s">
-        <v>200</v>
       </c>
       <c r="C62" s="4">
         <v>1</v>
@@ -2013,7 +2025,7 @@
         <v>59</v>
       </c>
       <c r="C78" s="4" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="H78" s="1" t="s">
         <v>64</v>
@@ -2034,8 +2046,15 @@
       </c>
     </row>
     <row r="80" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="1"/>
-      <c r="C80" s="1"/>
+      <c r="A80" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="B80" s="27" t="s">
+        <v>59</v>
+      </c>
+      <c r="C80" s="4" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="81" s="1" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="82" s="1" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2116,7 +2135,7 @@
         <v>0.5</v>
       </c>
       <c r="H102" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="103" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -2130,7 +2149,7 @@
         <v>0.5</v>
       </c>
       <c r="H103" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="104" spans="1:8" ht="9" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2176,7 +2195,7 @@
         <v>35</v>
       </c>
       <c r="C125" s="19" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D125" s="18" t="s">
         <v>87</v>
@@ -2185,7 +2204,7 @@
     </row>
     <row r="126" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A126" s="2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B126" s="26" t="s">
         <v>35</v>
@@ -2225,13 +2244,13 @@
         <v>35</v>
       </c>
       <c r="C128" s="19" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="D128" s="18" t="s">
         <v>87</v>
       </c>
       <c r="H128" s="11" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="129" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2242,7 +2261,7 @@
         <v>35</v>
       </c>
       <c r="C129" s="19" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D129" s="18" t="s">
         <v>87</v>
@@ -2277,7 +2296,7 @@
         <v>35</v>
       </c>
       <c r="C131" s="19" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D131" s="18" t="s">
         <v>87</v>
@@ -2330,7 +2349,7 @@
     </row>
     <row r="135" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A135" s="2" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="B135" s="26" t="s">
         <v>35</v>
@@ -2342,13 +2361,13 @@
     </row>
     <row r="136" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A136" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B136" s="26" t="s">
         <v>35</v>
       </c>
       <c r="C136" s="19" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="D136" s="18" t="s">
         <v>87</v>
@@ -2357,13 +2376,13 @@
     </row>
     <row r="137" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A137" s="2" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="B137" s="26" t="s">
         <v>35</v>
       </c>
       <c r="C137" s="19" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D137" s="18" t="s">
         <v>87</v>
@@ -2371,110 +2390,119 @@
     </row>
     <row r="138" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A138" s="2" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="B138" s="26" t="s">
         <v>35</v>
       </c>
       <c r="C138" s="19" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="139" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A139" s="2" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="B139" s="26" t="s">
         <v>35</v>
       </c>
       <c r="C139" s="19" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="140" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A140" s="2" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="B140" s="26" t="s">
         <v>35</v>
       </c>
       <c r="C140" s="19" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="141" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A141" s="2" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="B141" s="26" t="s">
         <v>35</v>
       </c>
       <c r="C141" s="19" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="142" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A142" s="2" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="B142" s="26" t="s">
         <v>35</v>
       </c>
       <c r="C142" s="19" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
     </row>
     <row r="143" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A143" s="2" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="B143" s="26" t="s">
         <v>35</v>
       </c>
       <c r="C143" s="19" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
     </row>
     <row r="144" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A144" s="2" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B144" s="26" t="s">
         <v>35</v>
       </c>
       <c r="C144" s="19" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="145" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A145" s="2" t="s">
         <v>260</v>
-      </c>
-    </row>
-    <row r="145" spans="1:3" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A145" s="2" t="s">
-        <v>262</v>
       </c>
       <c r="B145" s="26" t="s">
         <v>35</v>
       </c>
       <c r="C145" s="19"/>
     </row>
-    <row r="146" spans="1:3" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C146" s="40"/>
-    </row>
-    <row r="147" spans="1:3" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="148" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="149" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="150" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="151" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="152" spans="1:3" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="153" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="154" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="155" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="156" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="157" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="158" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="159" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="160" spans="1:3" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="146" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A146" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="B146" s="26" t="s">
+        <v>35</v>
+      </c>
+      <c r="C146" s="19"/>
+      <c r="H146" s="1" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="147" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="148" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="149" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="150" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="151" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="152" spans="1:8" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="153" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="154" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="155" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="156" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="157" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="158" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="159" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="160" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="161" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A161" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B161" s="26" t="s">
         <v>35</v>
@@ -2483,7 +2511,7 @@
     </row>
     <row r="162" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A162" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B162" s="26" t="s">
         <v>35</v>
@@ -2492,7 +2520,7 @@
     </row>
     <row r="163" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A163" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C163" s="1"/>
       <c r="E163" s="25" t="s">
@@ -2502,12 +2530,12 @@
         <v>4</v>
       </c>
       <c r="H163" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="164" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A164" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E164" s="25" t="s">
         <v>0</v>
@@ -2516,13 +2544,13 @@
         <v>0.5</v>
       </c>
       <c r="H164" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="165" spans="1:8" ht="13.9" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="166" spans="1:8" s="35" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A166" s="32" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B166" s="33"/>
       <c r="C166" s="34"/>
@@ -2591,7 +2619,7 @@
     </row>
     <row r="170" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A170" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B170" s="26" t="s">
         <v>35</v>
@@ -2607,12 +2635,12 @@
         <v>0</v>
       </c>
       <c r="H170" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="171" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A171" s="2" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B171" s="26" t="s">
         <v>35</v>
@@ -2630,7 +2658,7 @@
     </row>
     <row r="172" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A172" s="2" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B172" s="26" t="s">
         <v>35</v>
@@ -2681,7 +2709,7 @@
         <v>35</v>
       </c>
       <c r="C182" s="19" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D182" s="18" t="s">
         <v>87</v>
@@ -2701,7 +2729,7 @@
         <v>35</v>
       </c>
       <c r="C183" s="19" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D183" s="18" t="s">
         <v>87</v>
@@ -2724,7 +2752,7 @@
         <v>35</v>
       </c>
       <c r="C184" s="19" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D184" s="18" t="s">
         <v>87</v>
@@ -2744,7 +2772,7 @@
         <v>35</v>
       </c>
       <c r="C185" s="19" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D185" s="18" t="s">
         <v>87</v>
@@ -2782,7 +2810,7 @@
         <v>35</v>
       </c>
       <c r="C187" s="19" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D187" s="18" t="s">
         <v>87</v>
@@ -2796,7 +2824,7 @@
     </row>
     <row r="188" spans="1:8" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A188" s="2" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B188" s="26" t="s">
         <v>35</v>
@@ -2839,7 +2867,7 @@
         <v>100000</v>
       </c>
       <c r="H205" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="206" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2929,7 +2957,7 @@
         <v>0</v>
       </c>
       <c r="E226" s="6" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="F226" s="4" t="b">
         <v>1</v>
@@ -2939,11 +2967,11 @@
       </c>
     </row>
     <row r="227" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A227" s="43" t="s">
+      <c r="A227" s="42" t="s">
         <v>51</v>
       </c>
       <c r="B227" s="6" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C227" s="4" t="b">
         <v>1</v>
@@ -2952,7 +2980,7 @@
         <v>1</v>
       </c>
       <c r="E227" s="6" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F227" s="4" t="b">
         <v>1</v>
@@ -2962,7 +2990,7 @@
       </c>
     </row>
     <row r="228" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A228" s="43"/>
+      <c r="A228" s="42"/>
       <c r="B228" s="6" t="s">
         <v>21</v>
       </c>
@@ -2983,7 +3011,7 @@
       </c>
     </row>
     <row r="229" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A229" s="43"/>
+      <c r="A229" s="42"/>
       <c r="B229" s="6" t="s">
         <v>148</v>
       </c>
@@ -3004,7 +3032,7 @@
       </c>
     </row>
     <row r="230" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A230" s="43"/>
+      <c r="A230" s="42"/>
       <c r="B230" s="6" t="s">
         <v>130</v>
       </c>
@@ -3025,7 +3053,7 @@
       </c>
     </row>
     <row r="231" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A231" s="43"/>
+      <c r="A231" s="42"/>
       <c r="B231" s="6" t="s">
         <v>5</v>
       </c>
@@ -3046,7 +3074,7 @@
       </c>
     </row>
     <row r="232" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A232" s="43"/>
+      <c r="A232" s="42"/>
       <c r="B232" s="6" t="s">
         <v>151</v>
       </c>
@@ -3067,7 +3095,7 @@
       </c>
     </row>
     <row r="233" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A233" s="43"/>
+      <c r="A233" s="42"/>
       <c r="B233" s="6" t="s">
         <v>30</v>
       </c>
@@ -3088,7 +3116,7 @@
       </c>
     </row>
     <row r="234" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A234" s="43"/>
+      <c r="A234" s="42"/>
       <c r="B234" s="6" t="s">
         <v>16</v>
       </c>
@@ -3109,7 +3137,7 @@
       </c>
     </row>
     <row r="235" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A235" s="43"/>
+      <c r="A235" s="42"/>
       <c r="B235" s="6" t="s">
         <v>6</v>
       </c>
@@ -3130,7 +3158,7 @@
       </c>
     </row>
     <row r="236" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A236" s="43"/>
+      <c r="A236" s="42"/>
       <c r="B236" s="6" t="s">
         <v>8</v>
       </c>
@@ -3151,7 +3179,7 @@
       </c>
     </row>
     <row r="237" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A237" s="43"/>
+      <c r="A237" s="42"/>
       <c r="B237" s="6" t="s">
         <v>7</v>
       </c>
@@ -3172,7 +3200,7 @@
       </c>
     </row>
     <row r="238" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A238" s="43"/>
+      <c r="A238" s="42"/>
       <c r="B238" s="6" t="s">
         <v>9</v>
       </c>
@@ -3193,7 +3221,7 @@
       </c>
     </row>
     <row r="239" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A239" s="43"/>
+      <c r="A239" s="42"/>
       <c r="B239" s="6" t="s">
         <v>11</v>
       </c>
@@ -3214,7 +3242,7 @@
       </c>
     </row>
     <row r="240" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A240" s="43"/>
+      <c r="A240" s="42"/>
       <c r="B240" s="6" t="s">
         <v>12</v>
       </c>
@@ -3235,7 +3263,7 @@
       </c>
     </row>
     <row r="241" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A241" s="43"/>
+      <c r="A241" s="42"/>
       <c r="B241" s="6" t="s">
         <v>27</v>
       </c>
@@ -3316,7 +3344,7 @@
       </c>
     </row>
     <row r="245" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A245" s="46" t="s">
+      <c r="A245" s="45" t="s">
         <v>169</v>
       </c>
       <c r="B245" s="6" t="s">
@@ -3339,7 +3367,7 @@
       </c>
     </row>
     <row r="246" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A246" s="46"/>
+      <c r="A246" s="45"/>
       <c r="B246" s="6" t="s">
         <v>157</v>
       </c>
@@ -3503,7 +3531,7 @@
     </row>
     <row r="299" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A299" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C299" s="28" t="s">
         <v>4</v>
@@ -3558,7 +3586,7 @@
     </row>
     <row r="305" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A305" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C305" s="28" t="s">
         <v>4</v>
@@ -3575,7 +3603,7 @@
         <v>1</v>
       </c>
       <c r="E306" s="22" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="F306" s="21" t="b">
         <v>1</v>
@@ -3589,7 +3617,7 @@
         <v>1</v>
       </c>
       <c r="E307" s="22" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="F307" s="21" t="b">
         <v>1</v>
@@ -3603,7 +3631,7 @@
         <v>1</v>
       </c>
       <c r="E308" s="22" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="F308" s="21" t="b">
         <v>1</v>
@@ -3617,7 +3645,7 @@
         <v>0</v>
       </c>
       <c r="E309" s="22" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="F309" s="21" t="b">
         <v>1</v>
@@ -3631,7 +3659,7 @@
         <v>1</v>
       </c>
       <c r="E310" s="22" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F310" s="21" t="b">
         <v>1</v>
@@ -3645,7 +3673,7 @@
         <v>1</v>
       </c>
       <c r="E311" s="22" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F311" s="21" t="b">
         <v>1</v>
@@ -3659,7 +3687,7 @@
         <v>0</v>
       </c>
       <c r="E312" s="22" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="F312" s="21" t="b">
         <v>1</v>
@@ -3673,7 +3701,7 @@
         <v>0</v>
       </c>
       <c r="E313" s="22" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="F313" s="21" t="b">
         <v>0</v>
@@ -3687,7 +3715,7 @@
         <v>0</v>
       </c>
       <c r="E314" s="22" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F314" s="21" t="b">
         <v>0</v>
@@ -3701,7 +3729,7 @@
         <v>0</v>
       </c>
       <c r="E315" s="22" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F315" s="21" t="b">
         <v>0</v>
@@ -3715,7 +3743,7 @@
         <v>1</v>
       </c>
       <c r="E316" s="22" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F316" s="21" t="b">
         <v>0</v>
@@ -3729,7 +3757,7 @@
         <v>1</v>
       </c>
       <c r="E317" s="22" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F317" s="21" t="b">
         <v>0</v>
@@ -3743,7 +3771,7 @@
         <v>1</v>
       </c>
       <c r="E318" s="22" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="F318" s="21" t="b">
         <v>0</v>
@@ -3757,7 +3785,7 @@
         <v>0</v>
       </c>
       <c r="E319" s="22" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="F319" s="21" t="b">
         <v>0</v>
@@ -3771,7 +3799,7 @@
         <v>0</v>
       </c>
       <c r="E320" s="22" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="F320" s="21" t="b">
         <v>0</v>
@@ -3779,13 +3807,13 @@
     </row>
     <row r="321" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B321" s="22" t="s">
+        <v>231</v>
+      </c>
+      <c r="C321" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="E321" s="22" t="s">
         <v>232</v>
-      </c>
-      <c r="C321" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="E321" s="22" t="s">
-        <v>233</v>
       </c>
       <c r="F321" s="21" t="b">
         <v>0</v>
@@ -3793,7 +3821,7 @@
     </row>
     <row r="322" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E322" s="22" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="F322" s="21" t="b">
         <v>0</v>
@@ -3801,7 +3829,7 @@
     </row>
     <row r="325" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A325" s="2" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="330" spans="1:6" x14ac:dyDescent="0.25">
@@ -3864,7 +3892,7 @@
       <formula>NOT(ISERROR(SEARCH("TRUE",F313)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations xWindow="547" yWindow="733" count="35">
+  <dataValidations xWindow="547" yWindow="733" count="34">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Path the simulation directory" prompt="All inputs are saved in the so-called simulation directory, which includes, excel , gdx and pickle files together with the GAMS files._x000a__x000a_The path should be relative to this excel file. Use &quot;..&quot; to go up one folder. Folder separator can be either &quot;/&quot; or &quot;\&quot;" sqref="C34:D34" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
     <dataValidation type="date" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Start day of the simulation" prompt="This is the simulated day. It must be comprised within the range of dates provided within the data files." sqref="C57" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>1</formula1>
@@ -3907,8 +3935,7 @@
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Default transmission price" prompt="this default value will be applied to all transmission lines for which detailed data has not been found" sqref="F170" xr:uid="{B1B52813-ED56-4C3F-897E-A486B3F54EDC}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Defaut transmission price" prompt="This number should be set to at least 400 €/MWh, depending on the zone this value might be even higher" sqref="F170" xr:uid="{B493F26D-85F7-4F28-86F5-08E6BA578D3F}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Transmission price" prompt="Table with the times series for each line. The firs line should contain the name of the considered interconnection (e.g: &quot;BE -&gt; NL&quot;)" sqref="C170" xr:uid="{428C4A26-B19C-456A-AEA1-9C85EDE1AEE7}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Reserve down requirements" prompt="Path to the time series for each zone._x000a_The unit should be MW_x000a_If not provided, a standard formula is used to evaluate the reserve needs" sqref="C162" xr:uid="{094AD1A9-55C8-427E-B2FD-E6A9640F2346}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Reserve up requirements" prompt="Path to the time series for each zone._x000a_The unit should be MW_x000a_If not provided, a standard formula is used to evaluate the reserve needs" sqref="C161" xr:uid="{54B64FDA-AB14-4A05-907F-32559C9DD1CC}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Reserve up requirements" prompt="Path to the time series for each zone._x000a_The unit should be MW_x000a_If not provided, a standard formula is used to evaluate the reserve needs" sqref="C161:C162" xr:uid="{54B64FDA-AB14-4A05-907F-32559C9DD1CC}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Heating demand" prompt="expressed in MWh" sqref="C135" xr:uid="{F5C6CB55-A203-47FE-96B0-DC9C451014C9}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Demand for Hydrogen" prompt="Time series, expressed in MWh!" sqref="C137" xr:uid="{CA14712D-8AB1-47D5-9826-5119B72CD67D}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Default value (in EUR/t_co2)" prompt="In case no data file is provided. This single value is used for all the sets." sqref="F167:F172" xr:uid="{00000000-0002-0000-0000-00000B000000}"/>
@@ -3917,7 +3944,7 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xWindow="547" yWindow="733" count="9">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xWindow="547" yWindow="733" count="10">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000011000000}">
           <x14:formula1>
             <xm:f>Lists!$A$2:$A$3</xm:f>
@@ -3972,6 +3999,12 @@
           </x14:formula1>
           <xm:sqref>C101</xm:sqref>
         </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Transmission grid type" prompt="Market-based (NTC) or DC power flow" xr:uid="{F2E7DC41-A5E6-4EFE-AA53-AA90C723D885}">
+          <x14:formula1>
+            <xm:f>Lists!$G$2:$G$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>C80</xm:sqref>
+        </x14:dataValidation>
       </x14:dataValidations>
     </ext>
   </extLst>
@@ -3981,22 +4014,24 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.7109375" customWidth="1"/>
     <col min="2" max="2" width="32.5703125" customWidth="1"/>
     <col min="3" max="3" width="21" customWidth="1"/>
     <col min="4" max="4" width="20" customWidth="1"/>
-    <col min="5" max="5" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23" customWidth="1"/>
+    <col min="6" max="6" width="31.7109375" customWidth="1"/>
+    <col min="7" max="7" width="25.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="16" t="s">
         <v>4</v>
       </c>
@@ -4015,8 +4050,11 @@
       <c r="F1" s="16" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1" s="16" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="b">
         <v>1</v>
       </c>
@@ -4035,8 +4073,11 @@
       <c r="F2" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="b">
         <v>0</v>
       </c>
@@ -4044,7 +4085,7 @@
         <v>43</v>
       </c>
       <c r="C3" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D3" t="s">
         <v>83</v>
@@ -4055,13 +4096,16 @@
       <c r="F3" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G3" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>44</v>
       </c>
       <c r="C4" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D4" t="s">
         <v>80</v>
@@ -4070,18 +4114,18 @@
         <v>139</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>129</v>
       </c>
       <c r="C5" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D5" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>132</v>
       </c>
@@ -4101,7 +4145,7 @@
       <selection sqref="A1:O16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="16"/>
   </cols>

</xml_diff>

<commit_message>
fix(GAMS): EQ_BS_Balance2 ill defined. Avoid in-feasibilities when ENS. Proper SectorXInitial value assigned inside rolling horizon.
</commit_message>
<xml_diff>
--- a/ConfigFiles/ConfigTestBoundarySector.xlsx
+++ b/ConfigFiles/ConfigTestBoundarySector.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26529"/>
   <workbookPr updateLinks="never" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\Github\Dispa-SET.git\ConfigFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{740A5B4E-DE1D-4749-B35F-1833C2414B22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF1A0B8E-21FF-44AE-9939-4DB54BAA2DE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="263">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="263">
   <si>
     <t>Default value</t>
   </si>
@@ -1127,21 +1127,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="14">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="12">
     <dxf>
       <fill>
         <patternFill>
@@ -1249,9 +1235,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1289,9 +1275,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1324,26 +1310,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1376,26 +1345,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1572,8 +1524,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:H330"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A99" workbookViewId="0">
-      <selection activeCell="A145" sqref="A145"/>
+    <sheetView tabSelected="1" topLeftCell="A144" workbookViewId="0">
+      <selection activeCell="C187" sqref="C187"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2846,12 +2798,15 @@
       <c r="A206" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="C206" s="1"/>
+      <c r="B206" s="26" t="s">
+        <v>35</v>
+      </c>
+      <c r="C206" s="19"/>
       <c r="E206" s="25" t="s">
         <v>0</v>
       </c>
       <c r="F206" s="5">
-        <v>1499</v>
+        <v>1</v>
       </c>
       <c r="H206" s="1" t="s">
         <v>145</v>
@@ -3816,28 +3771,20 @@
     <mergeCell ref="A245:A246"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
-  <conditionalFormatting sqref="C226:D247 C79 C35:C36 F226:G247">
-    <cfRule type="containsText" dxfId="13" priority="11" operator="containsText" text="FALSE">
+  <conditionalFormatting sqref="C35:C36 C79 C226:D247 F226:G247">
+    <cfRule type="containsText" dxfId="11" priority="11" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",C35)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="12" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="10" priority="12" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",C35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C101">
-    <cfRule type="containsText" dxfId="11" priority="9" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="9" priority="9" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",C101)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="10" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="8" priority="10" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",C101)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F322 C306:C321">
-    <cfRule type="containsText" dxfId="9" priority="7" operator="containsText" text="FALSE">
-      <formula>NOT(ISERROR(SEARCH("FALSE",C306)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="8" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",C306)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C300:C303">
@@ -3848,20 +3795,20 @@
       <formula>NOT(ISERROR(SEARCH("TRUE",C300)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F306:F312">
-    <cfRule type="containsText" dxfId="5" priority="3" operator="containsText" text="FALSE">
+  <conditionalFormatting sqref="C306:C321">
+    <cfRule type="containsText" dxfId="5" priority="7" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",C306)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="4" priority="8" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",C306)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F306:F322">
+    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",F306)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="4" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",F306)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F313:F321">
-    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="FALSE">
-      <formula>NOT(ISERROR(SEARCH("FALSE",F313)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",F313)))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations xWindow="547" yWindow="733" count="35">

</xml_diff>

<commit_message>
fix(GAMS): StartUp and ShutDown costs now properly displayed, ConfigTest drop downs work again
</commit_message>
<xml_diff>
--- a/ConfigFiles/ConfigTestBoundarySector.xlsx
+++ b/ConfigFiles/ConfigTestBoundarySector.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr updateLinks="never" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\UMSS\Documents\Dispa-SET\ConfigFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\Github\Dispa-SET.git\ConfigFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCA30900-35ED-4218-8DDF-0F5F852491FA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15836C2B-666B-442E-AD09-D2FBA77A18AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23929" yWindow="-113" windowWidth="24267" windowHeight="13749" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="268">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="269">
   <si>
     <t>Default value</t>
   </si>
@@ -803,9 +803,6 @@
     <t>Value</t>
   </si>
   <si>
-    <t>CPLEX Setting</t>
-  </si>
-  <si>
     <t>Default</t>
   </si>
   <si>
@@ -837,6 +834,12 @@
   </si>
   <si>
     <t>tests/dummy_data/boundary_sector/BS_Spillage_cost.csv</t>
+  </si>
+  <si>
+    <t>CPLEX Settings</t>
+  </si>
+  <si>
+    <t>Aggressive</t>
   </si>
 </sst>
 </file>
@@ -996,7 +999,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1055,9 +1058,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -1135,7 +1135,175 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="14">
+  <dxfs count="38">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1248,9 +1416,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1288,9 +1456,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1323,26 +1491,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1375,26 +1526,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1571,36 +1705,36 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:H330"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A123" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C147" sqref="C147"/>
+    <sheetView tabSelected="1" topLeftCell="A101" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E143" sqref="E143"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="48.44140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.44140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="68.6640625" style="13" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.109375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="16.44140625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="15.6640625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="6.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="96.33203125" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.109375" style="1"/>
+    <col min="1" max="1" width="48.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.42578125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="68.7109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.42578125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="15.7109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="7.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="96.28515625" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="53.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="43" t="s">
+    <row r="1" spans="1:8" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="42" t="s">
         <v>237</v>
       </c>
-      <c r="B1" s="43"/>
-      <c r="C1" s="43"/>
-      <c r="D1" s="43"/>
-      <c r="E1" s="43"/>
-      <c r="F1" s="43"/>
-      <c r="G1" s="43"/>
-      <c r="H1" s="43"/>
-    </row>
-    <row r="2" spans="1:8" ht="13.95" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="42"/>
+      <c r="H1" s="42"/>
+    </row>
+    <row r="2" spans="1:8" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -1610,20 +1744,20 @@
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
     </row>
-    <row r="3" spans="1:8" ht="13.95" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="1:8" s="31" customFormat="1" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="30"/>
-      <c r="B4" s="44" t="s">
+    <row r="3" spans="1:8" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="1:8" s="30" customFormat="1" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="29"/>
+      <c r="B4" s="43" t="s">
         <v>56</v>
       </c>
-      <c r="C4" s="44"/>
-      <c r="D4" s="44"/>
-      <c r="E4" s="44"/>
-      <c r="F4" s="44"/>
-      <c r="G4" s="44"/>
-      <c r="H4" s="44"/>
-    </row>
-    <row r="5" spans="1:8" s="8" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C4" s="43"/>
+      <c r="D4" s="43"/>
+      <c r="E4" s="43"/>
+      <c r="F4" s="43"/>
+      <c r="G4" s="43"/>
+      <c r="H4" s="43"/>
+    </row>
+    <row r="5" spans="1:8" s="8" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="7"/>
       <c r="B5" s="15"/>
       <c r="C5" s="15"/>
@@ -1633,21 +1767,21 @@
       <c r="G5" s="15"/>
       <c r="H5" s="15"/>
     </row>
-    <row r="6" spans="1:8" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="36" t="s">
+    <row r="6" spans="1:8" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="35" t="s">
         <v>49</v>
       </c>
-      <c r="B6" s="41" t="s">
+      <c r="B6" s="40" t="s">
         <v>179</v>
       </c>
-      <c r="C6" s="41"/>
-      <c r="D6" s="41"/>
-      <c r="E6" s="41"/>
-      <c r="F6" s="41"/>
-      <c r="G6" s="41"/>
-      <c r="H6" s="41"/>
-    </row>
-    <row r="7" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C6" s="40"/>
+      <c r="D6" s="40"/>
+      <c r="E6" s="40"/>
+      <c r="F6" s="40"/>
+      <c r="G6" s="40"/>
+      <c r="H6" s="40"/>
+    </row>
+    <row r="7" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="12"/>
       <c r="C7" s="12"/>
       <c r="D7" s="12"/>
@@ -1656,7 +1790,7 @@
       <c r="G7" s="12"/>
       <c r="H7" s="12"/>
     </row>
-    <row r="8" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="12"/>
       <c r="C8" s="12"/>
       <c r="D8" s="12"/>
@@ -1665,7 +1799,7 @@
       <c r="G8" s="12"/>
       <c r="H8" s="12"/>
     </row>
-    <row r="9" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="12"/>
       <c r="C9" s="12"/>
       <c r="D9" s="12"/>
@@ -1674,7 +1808,7 @@
       <c r="G9" s="12"/>
       <c r="H9" s="12"/>
     </row>
-    <row r="10" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="12"/>
       <c r="C10" s="12"/>
       <c r="D10" s="12"/>
@@ -1683,7 +1817,7 @@
       <c r="G10" s="12"/>
       <c r="H10" s="12"/>
     </row>
-    <row r="11" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="12"/>
       <c r="C11" s="12"/>
       <c r="D11" s="12"/>
@@ -1692,7 +1826,7 @@
       <c r="G11" s="12"/>
       <c r="H11" s="12"/>
     </row>
-    <row r="12" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="12"/>
       <c r="C12" s="12"/>
       <c r="D12" s="12"/>
@@ -1701,7 +1835,7 @@
       <c r="G12" s="12"/>
       <c r="H12" s="12"/>
     </row>
-    <row r="13" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="12"/>
       <c r="C13" s="12"/>
       <c r="D13" s="12"/>
@@ -1710,7 +1844,7 @@
       <c r="G13" s="12"/>
       <c r="H13" s="12"/>
     </row>
-    <row r="14" spans="1:8" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="12"/>
       <c r="C14" s="12"/>
       <c r="D14" s="12"/>
@@ -1719,67 +1853,67 @@
       <c r="G14" s="12"/>
       <c r="H14" s="12"/>
     </row>
-    <row r="15" spans="1:8" s="35" customFormat="1" ht="15.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="32" t="s">
+    <row r="15" spans="1:8" s="34" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="31" t="s">
         <v>175</v>
       </c>
-      <c r="B15" s="33"/>
-      <c r="C15" s="34"/>
-      <c r="D15" s="33"/>
-      <c r="E15" s="33"/>
-      <c r="F15" s="33"/>
-      <c r="G15" s="33"/>
-      <c r="H15" s="33"/>
-    </row>
-    <row r="16" spans="1:8" ht="14.1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="32"/>
+      <c r="C15" s="33"/>
+      <c r="D15" s="32"/>
+      <c r="E15" s="32"/>
+      <c r="F15" s="32"/>
+      <c r="G15" s="32"/>
+      <c r="H15" s="32"/>
+    </row>
+    <row r="16" spans="1:8" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="B16" s="26"/>
-    </row>
-    <row r="17" spans="1:2" ht="14.1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="25"/>
+    </row>
+    <row r="17" spans="1:2" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="B17" s="27"/>
-    </row>
-    <row r="18" spans="1:2" ht="14.1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="26"/>
+    </row>
+    <row r="18" spans="1:2" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="B18" s="25"/>
-    </row>
-    <row r="19" spans="1:2" ht="5.35" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="20" spans="1:2" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="21" spans="1:2" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="22" spans="1:2" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="23" spans="1:2" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="24" spans="1:2" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="25" spans="1:2" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="26" spans="1:2" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="27" spans="1:2" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="28" spans="1:2" ht="12.05" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="29" spans="1:2" ht="12.7" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="30" spans="1:2" ht="15.05" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="31" spans="1:2" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="32" spans="1:2" ht="9.6999999999999993" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="33" spans="1:8" s="35" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="32" t="s">
+      <c r="B18" s="24"/>
+    </row>
+    <row r="19" spans="1:2" ht="5.45" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="20" spans="1:2" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="21" spans="1:2" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="22" spans="1:2" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="1:2" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="1:2" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="1:2" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="1:2" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="1:2" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="1:2" ht="12" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="1:2" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:2" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="1:2" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="1:2" ht="9.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="33" spans="1:8" s="34" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="31" t="s">
         <v>165</v>
       </c>
-      <c r="B33" s="33"/>
-      <c r="C33" s="34"/>
-      <c r="D33" s="33"/>
-      <c r="E33" s="33"/>
-      <c r="F33" s="33"/>
-      <c r="G33" s="33"/>
-      <c r="H33" s="33"/>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B33" s="32"/>
+      <c r="C33" s="33"/>
+      <c r="D33" s="32"/>
+      <c r="E33" s="32"/>
+      <c r="F33" s="32"/>
+      <c r="G33" s="32"/>
+      <c r="H33" s="32"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B34" s="26" t="s">
+      <c r="B34" s="25" t="s">
         <v>35</v>
       </c>
       <c r="C34" s="4" t="s">
@@ -1790,11 +1924,11 @@
         <v>66</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B35" s="27" t="s">
+      <c r="B35" s="26" t="s">
         <v>4</v>
       </c>
       <c r="C35" s="4" t="b">
@@ -1804,11 +1938,11 @@
         <v>67</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B36" s="27" t="s">
+      <c r="B36" s="26" t="s">
         <v>4</v>
       </c>
       <c r="C36" s="4" t="b">
@@ -1818,20 +1952,20 @@
         <v>68</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="B37" s="26" t="s">
+      <c r="B37" s="25" t="s">
         <v>85</v>
       </c>
       <c r="C37" s="4"/>
     </row>
-    <row r="38" spans="1:8" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:8" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="B38" s="26" t="s">
+      <c r="B38" s="25" t="s">
         <v>85</v>
       </c>
       <c r="C38" s="4"/>
@@ -1839,60 +1973,60 @@
         <v>87</v>
       </c>
     </row>
-    <row r="39" spans="1:8" ht="14.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:8" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>254</v>
       </c>
-      <c r="B39" s="25" t="s">
+      <c r="B39" s="24" t="s">
         <v>255</v>
       </c>
-      <c r="C39" s="40">
+      <c r="C39" s="39">
         <v>5.9999999999999995E-4</v>
       </c>
     </row>
-    <row r="40" spans="1:8" ht="14.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F40" s="2" t="s">
+    <row r="40" spans="1:8" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="B40" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="C40" s="4" t="s">
         <v>256</v>
       </c>
-      <c r="G40" s="27" t="s">
-        <v>59</v>
-      </c>
-      <c r="H40" s="4" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" ht="25.55" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="42" spans="1:8" ht="25.55" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="43" spans="1:8" ht="25.55" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="44" spans="1:8" ht="25.55" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="45" spans="1:8" ht="25.55" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="46" spans="1:8" ht="25.55" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="47" spans="1:8" ht="25.55" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="48" spans="1:8" ht="25.55" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="49" spans="1:8" ht="25.55" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="50" spans="1:8" ht="25.55" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="51" spans="1:8" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="52" spans="1:8" ht="26.3" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="53" spans="1:8" ht="25.55" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="54" spans="1:8" ht="27.7" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="55" spans="1:8" ht="13.95" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="56" spans="1:8" s="35" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="32" t="s">
+    </row>
+    <row r="41" spans="1:8" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="42" spans="1:8" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="43" spans="1:8" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="44" spans="1:8" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="45" spans="1:8" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="46" spans="1:8" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="47" spans="1:8" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="48" spans="1:8" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="49" spans="1:8" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="50" spans="1:8" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="51" spans="1:8" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="52" spans="1:8" ht="26.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="53" spans="1:8" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="54" spans="1:8" ht="27.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="55" spans="1:8" ht="13.9" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="56" spans="1:8" s="34" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="31" t="s">
         <v>164</v>
       </c>
-      <c r="B56" s="33"/>
-      <c r="C56" s="34"/>
-      <c r="D56" s="33"/>
-      <c r="E56" s="33"/>
-      <c r="F56" s="33"/>
-      <c r="G56" s="33"/>
-      <c r="H56" s="33"/>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B56" s="32"/>
+      <c r="C56" s="33"/>
+      <c r="D56" s="32"/>
+      <c r="E56" s="32"/>
+      <c r="F56" s="32"/>
+      <c r="G56" s="32"/>
+      <c r="H56" s="32"/>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B57" s="25" t="s">
+      <c r="B57" s="24" t="s">
         <v>37</v>
       </c>
       <c r="C57" s="17">
@@ -1902,11 +2036,11 @@
         <v>70</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B58" s="25" t="s">
+      <c r="B58" s="24" t="s">
         <v>37</v>
       </c>
       <c r="C58" s="17">
@@ -1916,11 +2050,11 @@
         <v>71</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B59" s="25" t="s">
+      <c r="B59" s="24" t="s">
         <v>46</v>
       </c>
       <c r="C59" s="4">
@@ -1930,71 +2064,71 @@
         <v>86</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B60" s="25" t="s">
+      <c r="B60" s="24" t="s">
         <v>46</v>
       </c>
       <c r="C60" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="B61" s="25" t="s">
+      <c r="B61" s="24" t="s">
         <v>199</v>
       </c>
       <c r="C61" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:8" ht="15.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:8" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="B62" s="25" t="s">
+      <c r="B62" s="24" t="s">
         <v>199</v>
       </c>
       <c r="C62" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:8" ht="68.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="64" spans="1:8" ht="68.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="65" spans="1:8" ht="68.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="66" spans="1:8" ht="68.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="67" spans="1:8" ht="68.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="68" spans="1:8" ht="68.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="69" spans="1:8" ht="68.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="70" spans="1:8" ht="68.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="71" spans="1:8" ht="68.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="72" spans="1:8" ht="12.7" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="73" spans="1:8" ht="15.05" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="74" spans="1:8" ht="15.05" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="75" spans="1:8" s="35" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A75" s="32" t="s">
+    <row r="63" spans="1:8" ht="68.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="64" spans="1:8" ht="68.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="65" spans="1:8" ht="68.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="66" spans="1:8" ht="68.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="67" spans="1:8" ht="68.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="68" spans="1:8" ht="68.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="69" spans="1:8" ht="68.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="70" spans="1:8" ht="68.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="71" spans="1:8" ht="68.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="72" spans="1:8" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="73" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="74" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="75" spans="1:8" s="34" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A75" s="31" t="s">
         <v>162</v>
       </c>
-      <c r="B75" s="33"/>
-      <c r="C75" s="34"/>
-      <c r="D75" s="33"/>
-      <c r="E75" s="33"/>
-      <c r="F75" s="33"/>
-      <c r="G75" s="33"/>
-      <c r="H75" s="33"/>
-    </row>
-    <row r="76" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="B75" s="32"/>
+      <c r="C75" s="33"/>
+      <c r="D75" s="32"/>
+      <c r="E75" s="32"/>
+      <c r="F75" s="32"/>
+      <c r="G75" s="32"/>
+      <c r="H75" s="32"/>
+    </row>
+    <row r="76" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="C76" s="1"/>
     </row>
-    <row r="77" spans="1:8" ht="15.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B77" s="27" t="s">
+      <c r="B77" s="26" t="s">
         <v>59</v>
       </c>
       <c r="C77" s="4" t="s">
@@ -2004,11 +2138,11 @@
         <v>63</v>
       </c>
     </row>
-    <row r="78" spans="1:8" ht="15.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="B78" s="27" t="s">
+      <c r="B78" s="26" t="s">
         <v>59</v>
       </c>
       <c r="C78" s="4" t="s">
@@ -2018,11 +2152,11 @@
         <v>64</v>
       </c>
     </row>
-    <row r="79" spans="1:8" ht="12.7" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="B79" s="27" t="s">
+      <c r="B79" s="26" t="s">
         <v>4</v>
       </c>
       <c r="C79" s="4" t="b">
@@ -2032,92 +2166,44 @@
         <v>65</v>
       </c>
     </row>
-    <row r="80" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="1"/>
       <c r="C80" s="1"/>
     </row>
-    <row r="81" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A81" s="1"/>
-      <c r="C81" s="1"/>
-    </row>
-    <row r="82" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A82" s="1"/>
-      <c r="C82" s="1"/>
-    </row>
-    <row r="83" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A83" s="1"/>
-      <c r="C83" s="1"/>
-    </row>
-    <row r="84" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A84" s="1"/>
-      <c r="C84" s="1"/>
-    </row>
-    <row r="85" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A85" s="1"/>
-      <c r="C85" s="1"/>
-    </row>
-    <row r="86" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A86" s="1"/>
-      <c r="C86" s="1"/>
-    </row>
-    <row r="87" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A87" s="1"/>
-      <c r="C87" s="1"/>
-    </row>
-    <row r="88" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A88" s="1"/>
-      <c r="C88" s="1"/>
-    </row>
-    <row r="89" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A89" s="1"/>
-      <c r="C89" s="1"/>
-    </row>
-    <row r="90" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A90" s="1"/>
-      <c r="C90" s="1"/>
-    </row>
-    <row r="91" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A91" s="1"/>
-      <c r="C91" s="1"/>
-    </row>
-    <row r="92" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A92" s="1"/>
-      <c r="C92" s="1"/>
-    </row>
-    <row r="93" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A93" s="1"/>
-      <c r="C93" s="1"/>
-    </row>
-    <row r="94" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A94" s="1"/>
-      <c r="C94" s="1"/>
-    </row>
-    <row r="95" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A95" s="1"/>
-      <c r="C95" s="1"/>
-    </row>
-    <row r="96" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A96" s="1"/>
-      <c r="C96" s="1"/>
-    </row>
-    <row r="97" spans="1:8" ht="13.95" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="98" spans="1:8" s="35" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A98" s="32" t="s">
+    <row r="81" s="1" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="82" s="1" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="83" s="1" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="84" s="1" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="85" s="1" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="86" s="1" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="87" s="1" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="88" s="1" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="89" s="1" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="90" s="1" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="91" s="1" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="92" s="1" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="93" s="1" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="94" s="1" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="95" s="1" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="96" s="1" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="97" spans="1:8" ht="13.9" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="98" spans="1:8" s="34" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A98" s="31" t="s">
         <v>169</v>
       </c>
-      <c r="B98" s="33"/>
-      <c r="C98" s="34"/>
-      <c r="D98" s="33"/>
-      <c r="E98" s="33"/>
-      <c r="F98" s="33"/>
-      <c r="G98" s="33"/>
-      <c r="H98" s="33"/>
-    </row>
-    <row r="99" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B98" s="32"/>
+      <c r="C98" s="33"/>
+      <c r="D98" s="32"/>
+      <c r="E98" s="32"/>
+      <c r="F98" s="32"/>
+      <c r="G98" s="32"/>
+      <c r="H98" s="32"/>
+    </row>
+    <row r="99" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="B99" s="27" t="s">
+      <c r="B99" s="26" t="s">
         <v>59</v>
       </c>
       <c r="C99" s="4" t="s">
@@ -2127,11 +2213,11 @@
         <v>137</v>
       </c>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="B100" s="27" t="s">
+      <c r="B100" s="26" t="s">
         <v>59</v>
       </c>
       <c r="C100" s="4" t="s">
@@ -2141,22 +2227,22 @@
         <v>161</v>
       </c>
     </row>
-    <row r="101" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="B101" s="27" t="s">
+      <c r="B101" s="26" t="s">
         <v>4</v>
       </c>
       <c r="C101" s="4" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="102" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A102" s="29" t="s">
+    <row r="102" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A102" s="28" t="s">
         <v>170</v>
       </c>
-      <c r="E102" s="25" t="s">
+      <c r="E102" s="24" t="s">
         <v>0</v>
       </c>
       <c r="F102" s="5">
@@ -2166,11 +2252,11 @@
         <v>195</v>
       </c>
     </row>
-    <row r="103" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A103" s="29" t="s">
+    <row r="103" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A103" s="28" t="s">
         <v>171</v>
       </c>
-      <c r="E103" s="25" t="s">
+      <c r="E103" s="24" t="s">
         <v>0</v>
       </c>
       <c r="F103" s="5">
@@ -2180,46 +2266,46 @@
         <v>194</v>
       </c>
     </row>
-    <row r="104" spans="1:8" ht="9.1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="105" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="106" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="107" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="108" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="109" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="110" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="111" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="112" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="113" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="114" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="115" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="116" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="117" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="118" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="119" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="120" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="121" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="122" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="123" spans="1:8" s="10" customFormat="1" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:8" ht="9.1999999999999993" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="105" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="106" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="107" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="108" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="109" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="110" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="111" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="112" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="113" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="114" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="115" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="116" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="117" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="118" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="119" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="120" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="121" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="122" spans="1:8" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="123" spans="1:8" s="10" customFormat="1" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A123" s="9"/>
       <c r="C123" s="14"/>
     </row>
-    <row r="124" spans="1:8" s="35" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A124" s="32" t="s">
+    <row r="124" spans="1:8" s="34" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A124" s="31" t="s">
         <v>163</v>
       </c>
-      <c r="B124" s="33"/>
-      <c r="C124" s="34"/>
-      <c r="D124" s="33"/>
-      <c r="E124" s="33"/>
-      <c r="F124" s="33"/>
-      <c r="G124" s="33"/>
-      <c r="H124" s="33"/>
-    </row>
-    <row r="125" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B124" s="32"/>
+      <c r="C124" s="33"/>
+      <c r="D124" s="32"/>
+      <c r="E124" s="32"/>
+      <c r="F124" s="32"/>
+      <c r="G124" s="32"/>
+      <c r="H124" s="32"/>
+    </row>
+    <row r="125" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A125" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B125" s="26" t="s">
+      <c r="B125" s="25" t="s">
         <v>35</v>
       </c>
       <c r="C125" s="19" t="s">
@@ -2230,18 +2316,18 @@
       </c>
       <c r="H125" s="11"/>
     </row>
-    <row r="126" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A126" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="B126" s="26" t="s">
+      <c r="B126" s="25" t="s">
         <v>35</v>
       </c>
       <c r="C126" s="19"/>
       <c r="D126" s="18" t="s">
         <v>87</v>
       </c>
-      <c r="E126" s="25" t="s">
+      <c r="E126" s="24" t="s">
         <v>0</v>
       </c>
       <c r="F126" s="5">
@@ -2249,14 +2335,14 @@
       </c>
       <c r="H126" s="11"/>
     </row>
-    <row r="127" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A127" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B127" s="26" t="s">
+      <c r="B127" s="25" t="s">
         <v>35</v>
       </c>
-      <c r="C127" s="23"/>
+      <c r="C127" s="22"/>
       <c r="D127" s="18" t="s">
         <v>87</v>
       </c>
@@ -2264,11 +2350,11 @@
         <v>52</v>
       </c>
     </row>
-    <row r="128" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A128" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B128" s="26" t="s">
+      <c r="B128" s="25" t="s">
         <v>35</v>
       </c>
       <c r="C128" s="19" t="s">
@@ -2281,11 +2367,11 @@
         <v>193</v>
       </c>
     </row>
-    <row r="129" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A129" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B129" s="26" t="s">
+      <c r="B129" s="25" t="s">
         <v>35</v>
       </c>
       <c r="C129" s="19" t="s">
@@ -2295,18 +2381,18 @@
         <v>87</v>
       </c>
     </row>
-    <row r="130" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A130" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B130" s="26" t="s">
+      <c r="B130" s="25" t="s">
         <v>35</v>
       </c>
       <c r="C130" s="19"/>
       <c r="D130" s="18" t="s">
         <v>87</v>
       </c>
-      <c r="E130" s="25" t="s">
+      <c r="E130" s="24" t="s">
         <v>0</v>
       </c>
       <c r="F130" s="5">
@@ -2316,11 +2402,11 @@
         <v>69</v>
       </c>
     </row>
-    <row r="131" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A131" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B131" s="26" t="s">
+      <c r="B131" s="25" t="s">
         <v>35</v>
       </c>
       <c r="C131" s="19" t="s">
@@ -2333,11 +2419,11 @@
         <v>53</v>
       </c>
     </row>
-    <row r="132" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A132" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="B132" s="26" t="s">
+      <c r="B132" s="25" t="s">
         <v>35</v>
       </c>
       <c r="C132" s="19"/>
@@ -2348,11 +2434,11 @@
         <v>54</v>
       </c>
     </row>
-    <row r="133" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A133" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="B133" s="26" t="s">
+      <c r="B133" s="25" t="s">
         <v>35</v>
       </c>
       <c r="C133" s="19"/>
@@ -2363,11 +2449,11 @@
         <v>55</v>
       </c>
     </row>
-    <row r="134" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A134" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="B134" s="26" t="s">
+      <c r="B134" s="25" t="s">
         <v>35</v>
       </c>
       <c r="C134" s="19"/>
@@ -2375,11 +2461,11 @@
         <v>87</v>
       </c>
     </row>
-    <row r="135" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A135" s="2" t="s">
-        <v>260</v>
-      </c>
-      <c r="B135" s="26" t="s">
+        <v>259</v>
+      </c>
+      <c r="B135" s="25" t="s">
         <v>35</v>
       </c>
       <c r="C135" s="19"/>
@@ -2387,11 +2473,11 @@
         <v>87</v>
       </c>
     </row>
-    <row r="136" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A136" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="B136" s="26" t="s">
+      <c r="B136" s="25" t="s">
         <v>35</v>
       </c>
       <c r="C136" s="19" t="s">
@@ -2402,11 +2488,11 @@
       </c>
       <c r="H136" s="11"/>
     </row>
-    <row r="137" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A137" s="2" t="s">
         <v>245</v>
       </c>
-      <c r="B137" s="26" t="s">
+      <c r="B137" s="25" t="s">
         <v>35</v>
       </c>
       <c r="C137" s="19" t="s">
@@ -2416,151 +2502,151 @@
         <v>87</v>
       </c>
     </row>
-    <row r="138" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A138" s="2" t="s">
         <v>238</v>
       </c>
-      <c r="B138" s="26" t="s">
+      <c r="B138" s="25" t="s">
         <v>35</v>
       </c>
       <c r="C138" s="19" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="139" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A139" s="2" t="s">
         <v>239</v>
       </c>
-      <c r="B139" s="26" t="s">
+      <c r="B139" s="25" t="s">
         <v>35</v>
       </c>
       <c r="C139" s="19" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="140" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A140" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="B140" s="26" t="s">
+      <c r="B140" s="25" t="s">
         <v>35</v>
       </c>
       <c r="C140" s="19" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="141" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A141" s="2" t="s">
         <v>241</v>
       </c>
-      <c r="B141" s="26" t="s">
+      <c r="B141" s="25" t="s">
         <v>35</v>
       </c>
       <c r="C141" s="19" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="142" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A142" s="2" t="s">
         <v>244</v>
       </c>
-      <c r="B142" s="26" t="s">
+      <c r="B142" s="25" t="s">
         <v>35</v>
       </c>
       <c r="C142" s="19" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="143" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A143" s="2" t="s">
         <v>252</v>
       </c>
-      <c r="B143" s="26" t="s">
+      <c r="B143" s="25" t="s">
         <v>35</v>
       </c>
       <c r="C143" s="19" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="144" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A144" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="B144" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="C144" s="19" t="s">
         <v>258</v>
       </c>
-      <c r="B144" s="26" t="s">
+    </row>
+    <row r="145" spans="1:3" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A145" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="B145" s="25" t="s">
         <v>35</v>
       </c>
-      <c r="C144" s="19" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="145" spans="1:3" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A145" s="2" t="s">
+      <c r="C145" s="19"/>
+    </row>
+    <row r="146" spans="1:3" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A146" s="2" t="s">
         <v>261</v>
       </c>
-      <c r="B145" s="26" t="s">
+      <c r="B146" s="25" t="s">
         <v>35</v>
       </c>
-      <c r="C145" s="19"/>
-    </row>
-    <row r="146" spans="1:3" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A146" s="2" t="s">
+      <c r="C146" s="19" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A147" s="2" t="s">
         <v>262</v>
       </c>
-      <c r="B146" s="26" t="s">
+      <c r="B147" s="25" t="s">
         <v>35</v>
       </c>
-      <c r="C146" s="19" t="s">
+      <c r="C147" s="19" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="147" spans="1:3" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A147" s="2" t="s">
-        <v>263</v>
-      </c>
-      <c r="B147" s="26" t="s">
-        <v>35</v>
-      </c>
-      <c r="C147" s="19" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="148" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="149" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="150" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="151" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="152" spans="1:3" ht="13.95" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="153" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="154" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="155" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="156" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="157" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="158" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="159" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="160" spans="1:3" ht="15.05" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="161" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:3" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="149" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="150" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="151" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="152" spans="1:3" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="153" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="154" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="155" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="156" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="157" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="158" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="159" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="160" spans="1:3" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="161" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A161" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="B161" s="26" t="s">
+      <c r="B161" s="25" t="s">
         <v>35</v>
       </c>
       <c r="C161" s="19"/>
     </row>
-    <row r="162" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A162" s="2" t="s">
         <v>207</v>
       </c>
-      <c r="B162" s="26" t="s">
+      <c r="B162" s="25" t="s">
         <v>35</v>
       </c>
       <c r="C162" s="19"/>
     </row>
-    <row r="163" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A163" s="2" t="s">
         <v>202</v>
       </c>
       <c r="C163" s="1"/>
-      <c r="E163" s="25" t="s">
+      <c r="E163" s="24" t="s">
         <v>0</v>
       </c>
       <c r="F163" s="5">
@@ -2570,11 +2656,11 @@
         <v>203</v>
       </c>
     </row>
-    <row r="164" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A164" s="2" t="s">
         <v>200</v>
       </c>
-      <c r="E164" s="25" t="s">
+      <c r="E164" s="24" t="s">
         <v>0</v>
       </c>
       <c r="F164" s="5">
@@ -2584,67 +2670,67 @@
         <v>201</v>
       </c>
     </row>
-    <row r="165" spans="1:8" ht="13.95" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="166" spans="1:8" s="35" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A166" s="32" t="s">
+    <row r="165" spans="1:8" ht="13.9" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="166" spans="1:8" s="34" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A166" s="31" t="s">
         <v>191</v>
       </c>
-      <c r="B166" s="33"/>
-      <c r="C166" s="34"/>
-      <c r="D166" s="33"/>
-      <c r="E166" s="33"/>
-      <c r="F166" s="33"/>
-      <c r="G166" s="33"/>
-      <c r="H166" s="33"/>
-    </row>
-    <row r="167" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B166" s="32"/>
+      <c r="C166" s="33"/>
+      <c r="D166" s="32"/>
+      <c r="E166" s="32"/>
+      <c r="F166" s="32"/>
+      <c r="G166" s="32"/>
+      <c r="H166" s="32"/>
+    </row>
+    <row r="167" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A167" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="B167" s="26" t="s">
+      <c r="B167" s="25" t="s">
         <v>35</v>
       </c>
       <c r="C167" s="19"/>
       <c r="D167" s="18" t="s">
         <v>87</v>
       </c>
-      <c r="E167" s="25" t="s">
+      <c r="E167" s="24" t="s">
         <v>0</v>
       </c>
       <c r="F167" s="5">
         <v>90</v>
       </c>
     </row>
-    <row r="168" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A168" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="B168" s="26" t="s">
+      <c r="B168" s="25" t="s">
         <v>35</v>
       </c>
       <c r="C168" s="19"/>
       <c r="D168" s="18" t="s">
         <v>87</v>
       </c>
-      <c r="E168" s="25" t="s">
+      <c r="E168" s="24" t="s">
         <v>0</v>
       </c>
       <c r="F168" s="5">
         <v>100</v>
       </c>
     </row>
-    <row r="169" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A169" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="B169" s="26" t="s">
+      <c r="B169" s="25" t="s">
         <v>35</v>
       </c>
       <c r="C169" s="19"/>
       <c r="D169" s="18" t="s">
         <v>87</v>
       </c>
-      <c r="E169" s="25" t="s">
+      <c r="E169" s="24" t="s">
         <v>0</v>
       </c>
       <c r="F169" s="5">
@@ -2654,18 +2740,18 @@
         <v>173</v>
       </c>
     </row>
-    <row r="170" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A170" s="2" t="s">
         <v>205</v>
       </c>
-      <c r="B170" s="26" t="s">
+      <c r="B170" s="25" t="s">
         <v>35</v>
       </c>
       <c r="C170" s="19"/>
       <c r="D170" s="18" t="s">
         <v>87</v>
       </c>
-      <c r="E170" s="25" t="s">
+      <c r="E170" s="24" t="s">
         <v>0</v>
       </c>
       <c r="F170" s="5">
@@ -2675,74 +2761,74 @@
         <v>206</v>
       </c>
     </row>
-    <row r="171" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A171" s="2" t="s">
         <v>246</v>
       </c>
-      <c r="B171" s="26" t="s">
+      <c r="B171" s="25" t="s">
         <v>35</v>
       </c>
       <c r="C171" s="19"/>
       <c r="D171" s="18" t="s">
         <v>87</v>
       </c>
-      <c r="E171" s="25" t="s">
+      <c r="E171" s="24" t="s">
         <v>0</v>
       </c>
       <c r="F171" s="5">
         <v>1000</v>
       </c>
     </row>
-    <row r="172" spans="1:8" ht="12.7" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A172" s="2" t="s">
         <v>234</v>
       </c>
-      <c r="B172" s="26" t="s">
+      <c r="B172" s="25" t="s">
         <v>35</v>
       </c>
       <c r="C172" s="19"/>
       <c r="D172" s="18" t="s">
         <v>87</v>
       </c>
-      <c r="E172" s="25" t="s">
+      <c r="E172" s="24" t="s">
         <v>0</v>
       </c>
       <c r="F172" s="5">
         <v>20</v>
       </c>
     </row>
-    <row r="173" spans="1:8" ht="12.7" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A173" s="1"/>
       <c r="C173" s="1"/>
     </row>
-    <row r="174" spans="1:8" ht="15.05" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="175" spans="1:8" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="176" spans="1:8" ht="11.3" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="177" spans="1:8" ht="12.05" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="178" spans="1:8" ht="12.7" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="179" spans="1:8" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="180" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="181" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="175" spans="1:8" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="176" spans="1:8" ht="11.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="177" spans="1:8" ht="12" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="178" spans="1:8" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="179" spans="1:8" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="180" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="181" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A181" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="B181" s="26" t="s">
+      <c r="B181" s="25" t="s">
         <v>35</v>
       </c>
       <c r="C181" s="19"/>
       <c r="D181" s="18"/>
-      <c r="E181" s="25" t="s">
+      <c r="E181" s="24" t="s">
         <v>0</v>
       </c>
       <c r="F181" s="5">
         <v>4</v>
       </c>
     </row>
-    <row r="182" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A182" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="B182" s="26" t="s">
+      <c r="B182" s="25" t="s">
         <v>35</v>
       </c>
       <c r="C182" s="19" t="s">
@@ -2751,18 +2837,18 @@
       <c r="D182" s="18" t="s">
         <v>87</v>
       </c>
-      <c r="E182" s="25" t="s">
+      <c r="E182" s="24" t="s">
         <v>0</v>
       </c>
       <c r="F182" s="5">
         <v>18</v>
       </c>
     </row>
-    <row r="183" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A183" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="B183" s="26" t="s">
+      <c r="B183" s="25" t="s">
         <v>35</v>
       </c>
       <c r="C183" s="19" t="s">
@@ -2771,7 +2857,7 @@
       <c r="D183" s="18" t="s">
         <v>87</v>
       </c>
-      <c r="E183" s="25" t="s">
+      <c r="E183" s="24" t="s">
         <v>0</v>
       </c>
       <c r="F183" s="5">
@@ -2781,11 +2867,11 @@
         <v>122</v>
       </c>
     </row>
-    <row r="184" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A184" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="B184" s="26" t="s">
+      <c r="B184" s="25" t="s">
         <v>35</v>
       </c>
       <c r="C184" s="19" t="s">
@@ -2794,18 +2880,18 @@
       <c r="D184" s="18" t="s">
         <v>87</v>
       </c>
-      <c r="E184" s="25" t="s">
+      <c r="E184" s="24" t="s">
         <v>0</v>
       </c>
       <c r="F184" s="5">
         <v>60</v>
       </c>
     </row>
-    <row r="185" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A185" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="B185" s="26" t="s">
+      <c r="B185" s="25" t="s">
         <v>35</v>
       </c>
       <c r="C185" s="19" t="s">
@@ -2814,36 +2900,36 @@
       <c r="D185" s="18" t="s">
         <v>87</v>
       </c>
-      <c r="E185" s="25" t="s">
+      <c r="E185" s="24" t="s">
         <v>0</v>
       </c>
       <c r="F185" s="5">
         <v>33</v>
       </c>
     </row>
-    <row r="186" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A186" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="B186" s="26" t="s">
+      <c r="B186" s="25" t="s">
         <v>35</v>
       </c>
       <c r="C186" s="19"/>
       <c r="D186" s="18" t="s">
         <v>87</v>
       </c>
-      <c r="E186" s="25" t="s">
+      <c r="E186" s="24" t="s">
         <v>0</v>
       </c>
       <c r="F186" s="5">
         <v>15</v>
       </c>
     </row>
-    <row r="187" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A187" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="B187" s="26" t="s">
+      <c r="B187" s="25" t="s">
         <v>35</v>
       </c>
       <c r="C187" s="19" t="s">
@@ -2852,87 +2938,87 @@
       <c r="D187" s="18" t="s">
         <v>87</v>
       </c>
-      <c r="E187" s="25" t="s">
+      <c r="E187" s="24" t="s">
         <v>0</v>
       </c>
       <c r="F187" s="5">
         <v>33</v>
       </c>
     </row>
-    <row r="188" spans="1:8" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:8" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A188" s="2" t="s">
         <v>235</v>
       </c>
-      <c r="B188" s="26" t="s">
+      <c r="B188" s="25" t="s">
         <v>35</v>
       </c>
       <c r="C188" s="19"/>
       <c r="D188" s="18" t="s">
         <v>87</v>
       </c>
-      <c r="E188" s="25" t="s">
+      <c r="E188" s="24" t="s">
         <v>0</v>
       </c>
       <c r="F188" s="5">
         <v>76</v>
       </c>
     </row>
-    <row r="190" spans="1:8" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="191" spans="1:8" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="192" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="193" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="194" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="195" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="196" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="197" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="198" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="199" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="200" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="201" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="202" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="203" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="204" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="205" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="191" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="192" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="193" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="194" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="195" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="196" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="197" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="198" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="199" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="200" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="201" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="202" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="203" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="204" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="205" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A205" s="2" t="s">
         <v>142</v>
       </c>
       <c r="C205" s="1"/>
-      <c r="E205" s="25" t="s">
-        <v>0</v>
-      </c>
-      <c r="F205" s="24">
+      <c r="E205" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="F205" s="23">
         <v>100000</v>
       </c>
       <c r="H205" s="1" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="206" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A206" s="2" t="s">
+        <v>265</v>
+      </c>
+      <c r="B206" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="C206" s="19" t="s">
         <v>266</v>
       </c>
-      <c r="B206" s="26" t="s">
-        <v>35</v>
-      </c>
-      <c r="C206" s="19" t="s">
-        <v>267</v>
-      </c>
-      <c r="E206" s="25" t="s">
+      <c r="E206" s="24" t="s">
         <v>0</v>
       </c>
       <c r="F206" s="5">
-        <v>1499</v>
+        <v>1</v>
       </c>
       <c r="H206" s="1" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="207" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A207" s="2" t="s">
         <v>143</v>
       </c>
       <c r="C207" s="1"/>
-      <c r="E207" s="25" t="s">
+      <c r="E207" s="24" t="s">
         <v>0</v>
       </c>
       <c r="F207" s="5">
@@ -2942,50 +3028,50 @@
         <v>145</v>
       </c>
     </row>
-    <row r="209" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="210" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="211" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="212" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="213" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="214" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="215" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="216" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="217" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="218" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="219" spans="1:3" ht="13.95" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="220" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="221" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="222" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="223" spans="1:3" ht="0.8" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="224" spans="1:3" s="10" customFormat="1" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="210" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="211" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="212" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="213" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="214" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="215" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="216" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="217" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="218" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="219" spans="1:3" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="220" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="221" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="222" spans="1:3" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="223" spans="1:3" ht="0.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="224" spans="1:3" s="10" customFormat="1" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A224" s="9"/>
       <c r="C224" s="14"/>
     </row>
-    <row r="225" spans="1:8" s="38" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A225" s="36" t="s">
+    <row r="225" spans="1:8" s="37" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A225" s="35" t="s">
         <v>166</v>
       </c>
-      <c r="B225" s="28" t="s">
+      <c r="B225" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="C225" s="36" t="s">
+      <c r="C225" s="35" t="s">
         <v>178</v>
       </c>
-      <c r="D225" s="39" t="s">
+      <c r="D225" s="38" t="s">
         <v>174</v>
       </c>
-      <c r="E225" s="28" t="s">
+      <c r="E225" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="F225" s="36" t="s">
+      <c r="F225" s="35" t="s">
         <v>178</v>
       </c>
-      <c r="G225" s="36" t="s">
+      <c r="G225" s="35" t="s">
         <v>174</v>
       </c>
-      <c r="H225" s="37"/>
-    </row>
-    <row r="226" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H225" s="36"/>
+    </row>
+    <row r="226" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A226" s="2" t="s">
         <v>50</v>
       </c>
@@ -3008,8 +3094,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="227" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A227" s="42" t="s">
+    <row r="227" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A227" s="41" t="s">
         <v>51</v>
       </c>
       <c r="B227" s="6" t="s">
@@ -3031,8 +3117,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="228" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A228" s="42"/>
+    <row r="228" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A228" s="41"/>
       <c r="B228" s="6" t="s">
         <v>21</v>
       </c>
@@ -3052,8 +3138,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="229" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A229" s="42"/>
+    <row r="229" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A229" s="41"/>
       <c r="B229" s="6" t="s">
         <v>147</v>
       </c>
@@ -3073,8 +3159,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="230" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A230" s="42"/>
+    <row r="230" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A230" s="41"/>
       <c r="B230" s="6" t="s">
         <v>130</v>
       </c>
@@ -3094,8 +3180,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="231" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A231" s="42"/>
+    <row r="231" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A231" s="41"/>
       <c r="B231" s="6" t="s">
         <v>5</v>
       </c>
@@ -3115,8 +3201,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="232" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A232" s="42"/>
+    <row r="232" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A232" s="41"/>
       <c r="B232" s="6" t="s">
         <v>150</v>
       </c>
@@ -3136,8 +3222,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="233" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A233" s="42"/>
+    <row r="233" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A233" s="41"/>
       <c r="B233" s="6" t="s">
         <v>30</v>
       </c>
@@ -3157,8 +3243,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="234" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A234" s="42"/>
+    <row r="234" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A234" s="41"/>
       <c r="B234" s="6" t="s">
         <v>16</v>
       </c>
@@ -3178,8 +3264,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="235" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A235" s="42"/>
+    <row r="235" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A235" s="41"/>
       <c r="B235" s="6" t="s">
         <v>6</v>
       </c>
@@ -3199,8 +3285,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="236" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A236" s="42"/>
+    <row r="236" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A236" s="41"/>
       <c r="B236" s="6" t="s">
         <v>8</v>
       </c>
@@ -3220,8 +3306,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="237" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A237" s="42"/>
+    <row r="237" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A237" s="41"/>
       <c r="B237" s="6" t="s">
         <v>7</v>
       </c>
@@ -3241,8 +3327,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="238" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A238" s="42"/>
+    <row r="238" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A238" s="41"/>
       <c r="B238" s="6" t="s">
         <v>9</v>
       </c>
@@ -3262,8 +3348,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="239" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A239" s="42"/>
+    <row r="239" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A239" s="41"/>
       <c r="B239" s="6" t="s">
         <v>11</v>
       </c>
@@ -3283,8 +3369,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="240" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A240" s="42"/>
+    <row r="240" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A240" s="41"/>
       <c r="B240" s="6" t="s">
         <v>12</v>
       </c>
@@ -3304,8 +3390,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="241" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A241" s="42"/>
+    <row r="241" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A241" s="41"/>
       <c r="B241" s="6" t="s">
         <v>27</v>
       </c>
@@ -3325,7 +3411,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="242" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B242" s="6" t="s">
         <v>13</v>
       </c>
@@ -3345,7 +3431,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="243" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B243" s="6" t="s">
         <v>14</v>
       </c>
@@ -3365,7 +3451,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="244" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B244" s="6" t="s">
         <v>19</v>
       </c>
@@ -3385,8 +3471,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="245" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A245" s="45" t="s">
+    <row r="245" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A245" s="44" t="s">
         <v>168</v>
       </c>
       <c r="B245" s="6" t="s">
@@ -3408,8 +3494,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="246" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A246" s="45"/>
+    <row r="246" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A246" s="44"/>
       <c r="B246" s="6" t="s">
         <v>156</v>
       </c>
@@ -3432,7 +3518,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="247" spans="1:8" ht="15.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="247" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B247" s="6" t="s">
         <v>15</v>
       </c>
@@ -3452,60 +3538,60 @@
         <v>0</v>
       </c>
     </row>
-    <row r="248" spans="1:8" ht="15.05" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="249" spans="1:8" ht="15.05" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="250" spans="1:8" ht="15.05" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="251" spans="1:8" ht="15.05" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="252" spans="1:8" ht="15.05" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="253" spans="1:8" ht="15.05" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="254" spans="1:8" ht="15.05" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="255" spans="1:8" ht="15.05" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="256" spans="1:8" ht="15.05" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="257" ht="15.05" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="258" ht="15.05" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="259" ht="15.05" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="260" ht="15.05" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="261" ht="15.05" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="262" ht="15.05" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="263" ht="15.05" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="264" ht="15.05" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="265" ht="15.05" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="266" ht="15.05" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="267" ht="15.05" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="268" ht="15.05" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="269" ht="15.05" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="270" ht="15.05" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="271" ht="15.05" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="272" ht="15.05" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="273" spans="1:8" ht="15.05" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="274" spans="1:8" s="35" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A274" s="32" t="s">
+    <row r="248" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="249" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="250" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="251" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="252" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="253" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="254" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="255" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="256" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="257" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="258" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="259" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="260" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="261" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="262" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="263" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="264" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="265" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="266" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="267" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="268" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="269" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="270" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="271" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="272" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="273" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="274" spans="1:8" s="34" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A274" s="31" t="s">
         <v>72</v>
       </c>
-      <c r="B274" s="33"/>
-      <c r="C274" s="34"/>
-      <c r="D274" s="33"/>
-      <c r="E274" s="33"/>
-      <c r="F274" s="33"/>
-      <c r="G274" s="33"/>
-      <c r="H274" s="33"/>
-    </row>
-    <row r="275" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B274" s="32"/>
+      <c r="C274" s="33"/>
+      <c r="D274" s="32"/>
+      <c r="E274" s="32"/>
+      <c r="F274" s="32"/>
+      <c r="G274" s="32"/>
+      <c r="H274" s="32"/>
+    </row>
+    <row r="275" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A275" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B275" s="25" t="s">
+      <c r="B275" s="24" t="s">
         <v>75</v>
       </c>
       <c r="C275" s="5">
         <v>0.16</v>
       </c>
     </row>
-    <row r="276" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="276" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A276" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="B276" s="25" t="s">
+      <c r="B276" s="24" t="s">
         <v>75</v>
       </c>
       <c r="C276" s="5">
@@ -3515,11 +3601,11 @@
         <v>77</v>
       </c>
     </row>
-    <row r="277" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="277" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A277" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="B277" s="25" t="s">
+      <c r="B277" s="24" t="s">
         <v>75</v>
       </c>
       <c r="C277" s="5">
@@ -3529,94 +3615,94 @@
         <v>78</v>
       </c>
     </row>
-    <row r="278" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="278" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A278" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="B278" s="25" t="s">
+      <c r="B278" s="24" t="s">
         <v>75</v>
       </c>
       <c r="C278" s="5">
         <v>1</v>
       </c>
     </row>
-    <row r="279" spans="1:8" ht="15.05" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="280" spans="1:8" ht="15.05" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="281" spans="1:8" ht="15.05" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="282" spans="1:8" ht="15.05" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="283" spans="1:8" ht="15.05" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="284" spans="1:8" ht="15.05" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="285" spans="1:8" ht="15.05" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="286" spans="1:8" ht="15.05" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="287" spans="1:8" ht="15.05" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="288" spans="1:8" ht="15.05" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="289" spans="1:8" ht="15.05" hidden="1" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="290" spans="1:8" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="291" spans="1:8" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="292" spans="1:8" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="293" spans="1:8" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="294" spans="1:8" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="295" spans="1:8" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="296" spans="1:8" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="297" spans="1:8" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="298" spans="1:8" s="8" customFormat="1" ht="15.65" x14ac:dyDescent="0.3">
-      <c r="A298" s="32" t="s">
+    <row r="279" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="280" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="281" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="282" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="283" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="284" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="285" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="286" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="287" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="288" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="289" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="290" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="291" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="292" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="293" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="294" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="295" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="296" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="297" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="298" spans="1:8" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A298" s="31" t="s">
         <v>167</v>
       </c>
-      <c r="B298" s="33"/>
-      <c r="C298" s="34"/>
-      <c r="D298" s="33"/>
-      <c r="E298" s="33"/>
-      <c r="F298" s="33"/>
-      <c r="G298" s="33"/>
-      <c r="H298" s="33"/>
-    </row>
-    <row r="299" spans="1:8" ht="15.65" x14ac:dyDescent="0.3">
+      <c r="B298" s="32"/>
+      <c r="C298" s="33"/>
+      <c r="D298" s="32"/>
+      <c r="E298" s="32"/>
+      <c r="F298" s="32"/>
+      <c r="G298" s="32"/>
+      <c r="H298" s="32"/>
+    </row>
+    <row r="299" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A299" s="2" t="s">
         <v>214</v>
       </c>
-      <c r="C299" s="28" t="s">
+      <c r="C299" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="D299" s="38"/>
-      <c r="E299" s="38"/>
-      <c r="F299" s="38"/>
-      <c r="G299" s="38"/>
-      <c r="H299" s="38"/>
-    </row>
-    <row r="300" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="D299" s="37"/>
+      <c r="E299" s="37"/>
+      <c r="F299" s="37"/>
+      <c r="G299" s="37"/>
+      <c r="H299" s="37"/>
+    </row>
+    <row r="300" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B300" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="C300" s="21" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="301" spans="1:8" ht="12.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C300" s="4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="301" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B301" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="C301" s="21" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="302" spans="1:8" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C301" s="4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="302" spans="1:8" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B302" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="C302" s="21" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="303" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C302" s="4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="303" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B303" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="C303" s="21" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="304" spans="1:8" s="38" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C303" s="4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="304" spans="1:8" s="37" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A304" s="2"/>
       <c r="B304" s="1"/>
       <c r="C304" s="13"/>
@@ -3626,255 +3712,255 @@
       <c r="G304" s="1"/>
       <c r="H304" s="1"/>
     </row>
-    <row r="305" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="305" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A305" s="2" t="s">
         <v>215</v>
       </c>
-      <c r="C305" s="28" t="s">
+      <c r="C305" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="F305" s="28" t="s">
+      <c r="F305" s="27" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="306" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B306" s="22" t="s">
+    <row r="306" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B306" s="21" t="s">
         <v>90</v>
       </c>
-      <c r="C306" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="E306" s="22" t="s">
+      <c r="C306" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="E306" s="21" t="s">
         <v>216</v>
       </c>
-      <c r="F306" s="21" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="307" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B307" s="22" t="s">
+      <c r="F306" s="4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="307" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B307" s="21" t="s">
         <v>91</v>
       </c>
-      <c r="C307" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="E307" s="22" t="s">
+      <c r="C307" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="E307" s="21" t="s">
         <v>217</v>
       </c>
-      <c r="F307" s="21" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="308" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B308" s="22" t="s">
+      <c r="F307" s="4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="308" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B308" s="21" t="s">
         <v>92</v>
       </c>
-      <c r="C308" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="E308" s="22" t="s">
+      <c r="C308" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="E308" s="21" t="s">
         <v>218</v>
       </c>
-      <c r="F308" s="21" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="309" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B309" s="22" t="s">
+      <c r="F308" s="4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="309" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B309" s="21" t="s">
         <v>93</v>
       </c>
-      <c r="C309" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="E309" s="22" t="s">
+      <c r="C309" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="E309" s="21" t="s">
         <v>219</v>
       </c>
-      <c r="F309" s="21" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="310" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B310" s="22" t="s">
+      <c r="F309" s="4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="310" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B310" s="21" t="s">
         <v>94</v>
       </c>
-      <c r="C310" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="E310" s="22" t="s">
+      <c r="C310" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="E310" s="21" t="s">
         <v>220</v>
       </c>
-      <c r="F310" s="21" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="311" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B311" s="22" t="s">
+      <c r="F310" s="4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="311" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B311" s="21" t="s">
         <v>95</v>
       </c>
-      <c r="C311" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="E311" s="22" t="s">
+      <c r="C311" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="E311" s="21" t="s">
         <v>221</v>
       </c>
-      <c r="F311" s="21" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="312" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B312" s="22" t="s">
+      <c r="F311" s="4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="312" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B312" s="21" t="s">
         <v>96</v>
       </c>
-      <c r="C312" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="E312" s="22" t="s">
+      <c r="C312" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="E312" s="21" t="s">
         <v>222</v>
       </c>
-      <c r="F312" s="21" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="313" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B313" s="22" t="s">
+      <c r="F312" s="4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="313" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B313" s="21" t="s">
         <v>97</v>
       </c>
-      <c r="C313" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="E313" s="22" t="s">
+      <c r="C313" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="E313" s="21" t="s">
         <v>223</v>
       </c>
-      <c r="F313" s="21" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="314" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B314" s="22" t="s">
+      <c r="F313" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="314" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B314" s="21" t="s">
         <v>98</v>
       </c>
-      <c r="C314" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="E314" s="22" t="s">
+      <c r="C314" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="E314" s="21" t="s">
         <v>224</v>
       </c>
-      <c r="F314" s="21" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="315" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B315" s="22" t="s">
+      <c r="F314" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="315" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B315" s="21" t="s">
         <v>99</v>
       </c>
-      <c r="C315" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="E315" s="22" t="s">
+      <c r="C315" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="E315" s="21" t="s">
         <v>225</v>
       </c>
-      <c r="F315" s="21" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="316" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B316" s="22" t="s">
+      <c r="F315" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="316" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B316" s="21" t="s">
         <v>100</v>
       </c>
-      <c r="C316" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="E316" s="22" t="s">
+      <c r="C316" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="E316" s="21" t="s">
         <v>226</v>
       </c>
-      <c r="F316" s="21" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="317" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B317" s="22" t="s">
+      <c r="F316" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="317" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B317" s="21" t="s">
         <v>101</v>
       </c>
-      <c r="C317" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="E317" s="22" t="s">
+      <c r="C317" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="E317" s="21" t="s">
         <v>227</v>
       </c>
-      <c r="F317" s="21" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="318" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B318" s="22" t="s">
+      <c r="F317" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="318" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B318" s="21" t="s">
         <v>102</v>
       </c>
-      <c r="C318" s="21" t="b">
-        <v>1</v>
-      </c>
-      <c r="E318" s="22" t="s">
+      <c r="C318" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="E318" s="21" t="s">
         <v>228</v>
       </c>
-      <c r="F318" s="21" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="319" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B319" s="22" t="s">
+      <c r="F318" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="319" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B319" s="21" t="s">
         <v>103</v>
       </c>
-      <c r="C319" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="E319" s="22" t="s">
+      <c r="C319" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="E319" s="21" t="s">
         <v>229</v>
       </c>
-      <c r="F319" s="21" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="320" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B320" s="22" t="s">
+      <c r="F319" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="320" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B320" s="21" t="s">
         <v>104</v>
       </c>
-      <c r="C320" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="E320" s="22" t="s">
+      <c r="C320" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="E320" s="21" t="s">
         <v>230</v>
       </c>
-      <c r="F320" s="21" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="321" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B321" s="22" t="s">
+      <c r="F320" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="321" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B321" s="21" t="s">
         <v>231</v>
       </c>
-      <c r="C321" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="E321" s="22" t="s">
+      <c r="C321" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="E321" s="21" t="s">
         <v>232</v>
       </c>
-      <c r="F321" s="21" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="322" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="E322" s="22" t="s">
+      <c r="F321" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="322" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E322" s="21" t="s">
         <v>233</v>
       </c>
-      <c r="F322" s="21" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="325" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F322" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="325" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A325" s="2" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="330" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="330" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F330" s="2"/>
     </row>
   </sheetData>
@@ -3886,52 +3972,116 @@
     <mergeCell ref="A245:A246"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="C226:D247 C79 C35:C36 F226:G247">
-    <cfRule type="containsText" dxfId="13" priority="11" operator="containsText" text="FALSE">
+  <conditionalFormatting sqref="C35:C36 C79 C227:D227 F226:G227">
+    <cfRule type="containsText" dxfId="37" priority="37" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",C35)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="12" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="36" priority="38" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",C35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C101">
-    <cfRule type="containsText" dxfId="11" priority="9" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="25" priority="25" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",C101)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="10" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="24" priority="26" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",C101)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F322 C306:C321">
-    <cfRule type="containsText" dxfId="9" priority="7" operator="containsText" text="FALSE">
+  <conditionalFormatting sqref="C300:C303">
+    <cfRule type="containsText" dxfId="23" priority="23" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",C300)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="22" priority="24" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",C300)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C306:C308">
+    <cfRule type="containsText" dxfId="21" priority="21" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",C306)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="8" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="20" priority="22" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",C306)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C300:C303">
-    <cfRule type="containsText" dxfId="7" priority="5" operator="containsText" text="FALSE">
-      <formula>NOT(ISERROR(SEARCH("FALSE",C300)))</formula>
+  <conditionalFormatting sqref="C310:C311">
+    <cfRule type="containsText" dxfId="19" priority="19" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",C310)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="6" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",C300)))</formula>
+    <cfRule type="containsText" dxfId="18" priority="20" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",C310)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C316:C318">
+    <cfRule type="containsText" dxfId="17" priority="17" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",C316)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="16" priority="18" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",C316)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F306:F312">
-    <cfRule type="containsText" dxfId="5" priority="3" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="15" priority="15" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",F306)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="4" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="14" priority="16" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",F306)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F313:F321">
-    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="FALSE">
+  <conditionalFormatting sqref="C309">
+    <cfRule type="containsText" dxfId="13" priority="13" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",C309)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="12" priority="14" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",C309)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C312:C315">
+    <cfRule type="containsText" dxfId="11" priority="11" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",C312)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="10" priority="12" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",C312)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C319:C321">
+    <cfRule type="containsText" dxfId="9" priority="9" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",C319)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="8" priority="10" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",C319)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F313:F322">
+    <cfRule type="containsText" dxfId="7" priority="7" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",F313)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="6" priority="8" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",F313)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C228:D247">
+    <cfRule type="containsText" dxfId="5" priority="5" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",C228)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="4" priority="6" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",C228)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F228:G247">
+    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",F228)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="2" priority="4" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",F228)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C226:D226">
+    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",C226)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",C226)))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations xWindow="547" yWindow="733" count="35">
@@ -3985,28 +4135,71 @@
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xWindow="547" yWindow="733" count="6">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{2208311D-42B6-4F60-9934-B08C9F1E5C51}">
+          <x14:formula1>
+            <xm:f>Lists!$G$2:$G$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>C40</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{A0CD96EF-65E1-4CDC-9807-E214C67B36DE}">
+          <x14:formula1>
+            <xm:f>Lists!$A$2:$A$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>C35:C36 C79 C101 C300:C303 C306:C321 F306:F322 F226:G247 C226:D247</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{184E1C98-F332-40AF-8944-4EE3B029C322}">
+          <x14:formula1>
+            <xm:f>Lists!$B$2:$B$6</xm:f>
+          </x14:formula1>
+          <xm:sqref>C77</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{F5BC13C8-E639-45F1-8901-CB963D4EE0E6}">
+          <x14:formula1>
+            <xm:f>Lists!$C$2:$C$5</xm:f>
+          </x14:formula1>
+          <xm:sqref>C78</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{A61AE642-9662-46F7-9E7E-D3A7DB5B5708}">
+          <x14:formula1>
+            <xm:f>Lists!$E$2:$E$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>C99</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{777CC868-04CE-4CC4-896B-21AD7CDCBDEF}">
+          <x14:formula1>
+            <xm:f>Lists!$F$2:$F$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>C100</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.6640625" customWidth="1"/>
-    <col min="2" max="2" width="32.5546875" customWidth="1"/>
-    <col min="3" max="3" width="21" customWidth="1"/>
-    <col min="4" max="4" width="20" customWidth="1"/>
-    <col min="5" max="5" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="16" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="16" t="s">
         <v>4</v>
       </c>
@@ -4025,8 +4218,11 @@
       <c r="F1" s="16" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G1" s="16" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="b">
         <v>1</v>
       </c>
@@ -4045,8 +4241,11 @@
       <c r="F2" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G2" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="b">
         <v>0</v>
       </c>
@@ -4065,8 +4264,11 @@
       <c r="F3" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G3" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>44</v>
       </c>
@@ -4080,7 +4282,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>129</v>
       </c>
@@ -4091,7 +4293,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>132</v>
       </c>
@@ -4111,12 +4313,12 @@
       <selection sqref="A1:O16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="16" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="16" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B1" s="16" t="s">
         <v>105</v>
       </c>
@@ -4160,7 +4362,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
         <v>90</v>
       </c>
@@ -4207,7 +4409,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="16" t="s">
         <v>91</v>
       </c>
@@ -4254,7 +4456,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
         <v>92</v>
       </c>
@@ -4301,7 +4503,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="16" t="s">
         <v>93</v>
       </c>
@@ -4348,7 +4550,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="16" t="s">
         <v>94</v>
       </c>
@@ -4395,7 +4597,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="16" t="s">
         <v>95</v>
       </c>
@@ -4442,7 +4644,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="16" t="s">
         <v>96</v>
       </c>
@@ -4489,7 +4691,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="16" t="s">
         <v>97</v>
       </c>
@@ -4536,7 +4738,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="16" t="s">
         <v>98</v>
       </c>
@@ -4583,7 +4785,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="16" t="s">
         <v>99</v>
       </c>
@@ -4630,7 +4832,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="16" t="s">
         <v>100</v>
       </c>
@@ -4677,7 +4879,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="16" t="s">
         <v>101</v>
       </c>
@@ -4724,7 +4926,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
         <v>102</v>
       </c>
@@ -4771,7 +4973,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="16" t="s">
         <v>103</v>
       </c>
@@ -4818,7 +5020,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="16" t="s">
         <v>104</v>
       </c>
@@ -4867,10 +5069,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:O16">
-    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="27" priority="1" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",B2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="26" priority="2" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",B2)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
fix(gams): startup and shudown costs properly displayed
</commit_message>
<xml_diff>
--- a/ConfigFiles/ConfigTestBoundarySector.xlsx
+++ b/ConfigFiles/ConfigTestBoundarySector.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\Github\Dispa-SET.git\ConfigFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15836C2B-666B-442E-AD09-D2FBA77A18AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6955EFC5-C45E-4E0D-9E47-0F9D1E886967}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1135,161 +1135,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="38">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="16">
     <dxf>
       <fill>
         <patternFill>
@@ -1706,7 +1552,7 @@
   <dimension ref="A1:H330"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A101" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E143" sqref="E143"/>
+      <selection activeCell="F127" sqref="F127"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2331,7 +2177,7 @@
         <v>0</v>
       </c>
       <c r="F126" s="5">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="H126" s="11"/>
     </row>
@@ -3972,116 +3818,60 @@
     <mergeCell ref="A245:A246"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="C35:C36 C79 C227:D227 F226:G227">
-    <cfRule type="containsText" dxfId="37" priority="37" operator="containsText" text="FALSE">
+  <conditionalFormatting sqref="C35:C36 C79">
+    <cfRule type="containsText" dxfId="15" priority="37" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",C35)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="36" priority="38" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="14" priority="38" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",C35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C101">
-    <cfRule type="containsText" dxfId="25" priority="25" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="13" priority="25" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",C101)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="24" priority="26" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="12" priority="26" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",C101)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C300:C303">
-    <cfRule type="containsText" dxfId="23" priority="23" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="11" priority="23" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",C300)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="22" priority="24" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="10" priority="24" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",C300)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C306:C308">
-    <cfRule type="containsText" dxfId="21" priority="21" operator="containsText" text="FALSE">
+  <conditionalFormatting sqref="C306:C321">
+    <cfRule type="containsText" dxfId="9" priority="9" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",C306)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="20" priority="22" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="8" priority="10" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",C306)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C310:C311">
-    <cfRule type="containsText" dxfId="19" priority="19" operator="containsText" text="FALSE">
-      <formula>NOT(ISERROR(SEARCH("FALSE",C310)))</formula>
+  <conditionalFormatting sqref="C226:D247">
+    <cfRule type="containsText" dxfId="7" priority="1" operator="containsText" text="FALSE">
+      <formula>NOT(ISERROR(SEARCH("FALSE",C226)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="18" priority="20" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",C310)))</formula>
+    <cfRule type="containsText" dxfId="6" priority="2" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",C226)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C316:C318">
-    <cfRule type="containsText" dxfId="17" priority="17" operator="containsText" text="FALSE">
-      <formula>NOT(ISERROR(SEARCH("FALSE",C316)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="16" priority="18" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",C316)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F306:F312">
-    <cfRule type="containsText" dxfId="15" priority="15" operator="containsText" text="FALSE">
+  <conditionalFormatting sqref="F306:F322">
+    <cfRule type="containsText" dxfId="5" priority="7" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",F306)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="14" priority="16" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="4" priority="8" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",F306)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C309">
-    <cfRule type="containsText" dxfId="13" priority="13" operator="containsText" text="FALSE">
-      <formula>NOT(ISERROR(SEARCH("FALSE",C309)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="14" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",C309)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C312:C315">
-    <cfRule type="containsText" dxfId="11" priority="11" operator="containsText" text="FALSE">
-      <formula>NOT(ISERROR(SEARCH("FALSE",C312)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="12" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",C312)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C319:C321">
-    <cfRule type="containsText" dxfId="9" priority="9" operator="containsText" text="FALSE">
-      <formula>NOT(ISERROR(SEARCH("FALSE",C319)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="10" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",C319)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F313:F322">
-    <cfRule type="containsText" dxfId="7" priority="7" operator="containsText" text="FALSE">
-      <formula>NOT(ISERROR(SEARCH("FALSE",F313)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="8" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",F313)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C228:D247">
-    <cfRule type="containsText" dxfId="5" priority="5" operator="containsText" text="FALSE">
-      <formula>NOT(ISERROR(SEARCH("FALSE",C228)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="6" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",C228)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F228:G247">
+  <conditionalFormatting sqref="F226:G247">
     <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="FALSE">
-      <formula>NOT(ISERROR(SEARCH("FALSE",F228)))</formula>
+      <formula>NOT(ISERROR(SEARCH("FALSE",F226)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="2" priority="4" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",F228)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C226:D226">
-    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="FALSE">
-      <formula>NOT(ISERROR(SEARCH("FALSE",C226)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",C226)))</formula>
+      <formula>NOT(ISERROR(SEARCH("TRUE",F226)))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations xWindow="547" yWindow="733" count="35">
@@ -5069,10 +4859,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:O16">
-    <cfRule type="containsText" dxfId="27" priority="1" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",B2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="26" priority="2" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",B2)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>